<commit_message>
Web Project Status Update
</commit_message>
<xml_diff>
--- a/Web Project Status.xlsx
+++ b/Web Project Status.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
-  <workbookPr autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-36740" yWindow="80" windowWidth="34620" windowHeight="21440"/>
+    <workbookView xWindow="-36735" yWindow="75" windowWidth="34620" windowHeight="16440"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -259,9 +259,6 @@
     <t>routed 10/29</t>
   </si>
   <si>
-    <t>awaiting slides</t>
-  </si>
-  <si>
     <t>CTOS PDS</t>
   </si>
   <si>
@@ -344,13 +341,16 @@
   </si>
   <si>
     <t>routed 11/04</t>
+  </si>
+  <si>
+    <t>Benji</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -414,8 +414,15 @@
       <color theme="11"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -432,6 +439,11 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
   </fills>
@@ -451,7 +463,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="25">
+  <cellStyleXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -477,8 +489,9 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -524,8 +537,10 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="1" xfId="25" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="1" xfId="25" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="25">
+  <cellStyles count="26">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -538,6 +553,7 @@
     <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Good" xfId="25" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -852,18 +868,18 @@
   <dimension ref="A1:X989"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="38.5" customWidth="1"/>
-    <col min="4" max="4" width="23.1640625" customWidth="1"/>
-    <col min="5" max="5" width="52.1640625" customWidth="1"/>
-    <col min="6" max="6" width="20.83203125" customWidth="1"/>
+    <col min="1" max="1" width="38.42578125" customWidth="1"/>
+    <col min="4" max="4" width="23.140625" customWidth="1"/>
+    <col min="5" max="5" width="52.140625" customWidth="1"/>
+    <col min="6" max="6" width="20.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="15.75" customHeight="1">
+    <row r="1" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -903,8 +919,8 @@
       <c r="W1" s="3"/>
       <c r="X1" s="3"/>
     </row>
-    <row r="2" spans="1:24" s="20" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A2" s="21" t="s">
+    <row r="2" spans="1:24" s="20" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="43" t="s">
         <v>8</v>
       </c>
       <c r="B2" s="22" t="s">
@@ -917,18 +933,18 @@
         <v>11</v>
       </c>
       <c r="E2" s="23" t="s">
+        <v>91</v>
+      </c>
+      <c r="F2" s="23" t="s">
         <v>92</v>
-      </c>
-      <c r="F2" s="23" t="s">
-        <v>93</v>
       </c>
       <c r="G2" s="24">
         <v>41936</v>
       </c>
     </row>
-    <row r="3" spans="1:24" s="20" customFormat="1" ht="15.75" customHeight="1">
+    <row r="3" spans="1:24" s="20" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="21" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B3" s="22" t="s">
         <v>12</v>
@@ -946,9 +962,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:24" s="20" customFormat="1" ht="12" customHeight="1">
+    <row r="4" spans="1:24" s="20" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="23" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B4" s="18"/>
       <c r="C4" s="17" t="s">
@@ -964,7 +980,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="5" spans="1:24" s="20" customFormat="1" ht="15.75" customHeight="1">
+    <row r="5" spans="1:24" s="20" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="21" t="s">
         <v>17</v>
       </c>
@@ -976,7 +992,7 @@
         <v>66</v>
       </c>
       <c r="E5" s="26" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F5" s="26" t="s">
         <v>19</v>
@@ -1002,7 +1018,7 @@
       <c r="W5" s="25"/>
       <c r="X5" s="25"/>
     </row>
-    <row r="6" spans="1:24" s="20" customFormat="1" ht="15.75" customHeight="1">
+    <row r="6" spans="1:24" s="20" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="17" t="s">
         <v>20</v>
       </c>
@@ -1014,7 +1030,7 @@
         <v>65</v>
       </c>
       <c r="E6" s="23" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F6" s="17" t="s">
         <v>22</v>
@@ -1040,7 +1056,7 @@
       <c r="W6" s="19"/>
       <c r="X6" s="19"/>
     </row>
-    <row r="7" spans="1:24" s="20" customFormat="1" ht="15.75" customHeight="1">
+    <row r="7" spans="1:24" s="20" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="17" t="s">
         <v>23</v>
       </c>
@@ -1052,7 +1068,7 @@
         <v>65</v>
       </c>
       <c r="E7" s="23" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F7" s="17" t="s">
         <v>25</v>
@@ -1076,7 +1092,7 @@
       <c r="W7" s="19"/>
       <c r="X7" s="19"/>
     </row>
-    <row r="8" spans="1:24" s="38" customFormat="1" ht="15.75" customHeight="1">
+    <row r="8" spans="1:24" s="38" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="36" t="s">
         <v>26</v>
       </c>
@@ -1085,27 +1101,27 @@
         <v>75</v>
       </c>
       <c r="E8" s="39" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F8" s="38" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:24" s="20" customFormat="1" ht="15.75" customHeight="1">
+    <row r="9" spans="1:24" s="20" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="17" t="s">
         <v>27</v>
       </c>
       <c r="D9" s="23" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E9" s="23" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F9" s="23" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:24" s="20" customFormat="1" ht="15.75" customHeight="1">
+    <row r="10" spans="1:24" s="20" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="17" t="s">
         <v>28</v>
       </c>
@@ -1116,13 +1132,13 @@
         <v>66</v>
       </c>
       <c r="E10" s="23" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F10" s="23" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="11" spans="1:24" s="38" customFormat="1" ht="15.75" customHeight="1">
+    <row r="11" spans="1:24" s="38" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="40" t="s">
         <v>30</v>
       </c>
@@ -1134,7 +1150,7 @@
         <v>66</v>
       </c>
       <c r="E11" s="42" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F11" s="41" t="s">
         <v>15</v>
@@ -1158,19 +1174,19 @@
       <c r="W11" s="41"/>
       <c r="X11" s="41"/>
     </row>
-    <row r="12" spans="1:24" ht="15.75" customHeight="1">
+    <row r="12" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B12" s="4"/>
       <c r="C12" s="7" t="s">
         <v>68</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F12" s="7" t="s">
         <v>54</v>
@@ -1194,7 +1210,7 @@
       <c r="W12" s="7"/>
       <c r="X12" s="7"/>
     </row>
-    <row r="13" spans="1:24" s="38" customFormat="1" ht="15.75" customHeight="1">
+    <row r="13" spans="1:24" s="38" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="40" t="s">
         <v>62</v>
       </c>
@@ -1205,13 +1221,13 @@
         <v>61</v>
       </c>
       <c r="E13" s="42" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F13" s="41" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:24" ht="15.75" customHeight="1">
+    <row r="14" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>64</v>
       </c>
@@ -1223,7 +1239,7 @@
         <v>66</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F14" s="7" t="s">
         <v>19</v>
@@ -1247,7 +1263,7 @@
       <c r="W14" s="7"/>
       <c r="X14" s="7"/>
     </row>
-    <row r="15" spans="1:24" ht="15.75" customHeight="1">
+    <row r="15" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>70</v>
       </c>
@@ -1281,7 +1297,7 @@
       <c r="W15" s="7"/>
       <c r="X15" s="7"/>
     </row>
-    <row r="16" spans="1:24" ht="15.75" customHeight="1">
+    <row r="16" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>71</v>
       </c>
@@ -1292,9 +1308,7 @@
       <c r="D16" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="E16" s="7" t="s">
-        <v>79</v>
-      </c>
+      <c r="E16" s="7"/>
       <c r="F16" s="7" t="s">
         <v>15</v>
       </c>
@@ -1319,7 +1333,7 @@
       <c r="W16" s="7"/>
       <c r="X16" s="7"/>
     </row>
-    <row r="17" spans="1:24" s="34" customFormat="1" ht="15.75" customHeight="1">
+    <row r="17" spans="1:24" s="34" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="33" t="s">
         <v>72</v>
       </c>
@@ -1331,7 +1345,7 @@
         <v>66</v>
       </c>
       <c r="E17" s="29" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F17" s="29" t="s">
         <v>69</v>
@@ -1355,7 +1369,7 @@
       <c r="W17" s="29"/>
       <c r="X17" s="29"/>
     </row>
-    <row r="18" spans="1:24" ht="15.75" customHeight="1">
+    <row r="18" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>73</v>
       </c>
@@ -1369,7 +1383,9 @@
       <c r="E18" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="F18" s="7"/>
+      <c r="F18" s="7" t="s">
+        <v>107</v>
+      </c>
       <c r="G18" s="7"/>
       <c r="H18" s="7"/>
       <c r="I18" s="7"/>
@@ -1389,22 +1405,22 @@
       <c r="W18" s="7"/>
       <c r="X18" s="7"/>
     </row>
-    <row r="19" spans="1:24" s="34" customFormat="1" ht="15.75" customHeight="1">
+    <row r="19" spans="1:24" s="34" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="33" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B19" s="33"/>
       <c r="C19" s="29" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D19" s="29" t="s">
         <v>75</v>
       </c>
       <c r="E19" s="29" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F19" s="29" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G19" s="35">
         <v>41948</v>
@@ -1427,16 +1443,16 @@
       <c r="W19" s="29"/>
       <c r="X19" s="29"/>
     </row>
-    <row r="20" spans="1:24" ht="15.75" customHeight="1">
+    <row r="20" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B20" s="4"/>
       <c r="C20" s="7" t="s">
         <v>68</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E20" s="7"/>
       <c r="F20" s="7"/>
@@ -1461,16 +1477,16 @@
       <c r="W20" s="7"/>
       <c r="X20" s="7"/>
     </row>
-    <row r="21" spans="1:24" ht="13">
+    <row r="21" spans="1:24" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B21" s="4"/>
       <c r="C21" s="7" t="s">
         <v>68</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E21" s="7"/>
       <c r="F21" s="7"/>
@@ -1493,15 +1509,15 @@
       <c r="W21" s="7"/>
       <c r="X21" s="7"/>
     </row>
-    <row r="22" spans="1:24" s="32" customFormat="1" ht="12">
+    <row r="22" spans="1:24" s="32" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A22" s="31" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B22" s="31"/>
       <c r="C22" s="31"/>
       <c r="D22" s="31"/>
       <c r="E22" s="31" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F22" s="31" t="s">
         <v>54</v>
@@ -1525,15 +1541,15 @@
       <c r="W22" s="31"/>
       <c r="X22" s="31"/>
     </row>
-    <row r="23" spans="1:24" s="32" customFormat="1" ht="12">
-      <c r="A23" s="31" t="s">
-        <v>88</v>
+    <row r="23" spans="1:24" s="32" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A23" s="44" t="s">
+        <v>87</v>
       </c>
       <c r="B23" s="31"/>
       <c r="C23" s="31"/>
       <c r="D23" s="31"/>
       <c r="E23" s="31" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F23" s="31" t="s">
         <v>54</v>
@@ -1557,15 +1573,15 @@
       <c r="W23" s="31"/>
       <c r="X23" s="31"/>
     </row>
-    <row r="24" spans="1:24" ht="12">
+    <row r="24" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A24" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B24" s="7"/>
       <c r="C24" s="7"/>
       <c r="D24" s="7"/>
       <c r="E24" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F24" s="7" t="s">
         <v>54</v>
@@ -1589,15 +1605,15 @@
       <c r="W24" s="7"/>
       <c r="X24" s="7"/>
     </row>
-    <row r="25" spans="1:24" ht="12">
+    <row r="25" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A25" s="7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B25" s="7"/>
       <c r="C25" s="7"/>
       <c r="D25" s="7"/>
       <c r="E25" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F25" s="7" t="s">
         <v>54</v>
@@ -1621,7 +1637,7 @@
       <c r="W25" s="7"/>
       <c r="X25" s="7"/>
     </row>
-    <row r="26" spans="1:24" ht="12">
+    <row r="26" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A26" s="7"/>
       <c r="B26" s="7"/>
       <c r="C26" s="7"/>
@@ -1647,7 +1663,7 @@
       <c r="W26" s="7"/>
       <c r="X26" s="7"/>
     </row>
-    <row r="27" spans="1:24" ht="12">
+    <row r="27" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A27" s="7"/>
       <c r="B27" s="7"/>
       <c r="C27" s="7"/>
@@ -1673,7 +1689,7 @@
       <c r="W27" s="7"/>
       <c r="X27" s="7"/>
     </row>
-    <row r="28" spans="1:24" ht="12">
+    <row r="28" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A28" s="7"/>
       <c r="B28" s="7"/>
       <c r="C28" s="7"/>
@@ -1699,7 +1715,7 @@
       <c r="W28" s="7"/>
       <c r="X28" s="7"/>
     </row>
-    <row r="29" spans="1:24" ht="12">
+    <row r="29" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A29" s="7"/>
       <c r="B29" s="7"/>
       <c r="C29" s="7"/>
@@ -1725,7 +1741,7 @@
       <c r="W29" s="7"/>
       <c r="X29" s="7"/>
     </row>
-    <row r="30" spans="1:24" ht="12">
+    <row r="30" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A30" s="7"/>
       <c r="B30" s="7"/>
       <c r="C30" s="7"/>
@@ -1751,7 +1767,7 @@
       <c r="W30" s="7"/>
       <c r="X30" s="7"/>
     </row>
-    <row r="31" spans="1:24" ht="12">
+    <row r="31" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A31" s="7"/>
       <c r="B31" s="7"/>
       <c r="C31" s="7"/>
@@ -1777,7 +1793,7 @@
       <c r="W31" s="7"/>
       <c r="X31" s="7"/>
     </row>
-    <row r="32" spans="1:24" ht="12">
+    <row r="32" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A32" s="7"/>
       <c r="B32" s="7"/>
       <c r="C32" s="7"/>
@@ -1803,7 +1819,7 @@
       <c r="W32" s="7"/>
       <c r="X32" s="7"/>
     </row>
-    <row r="33" spans="1:24" ht="12">
+    <row r="33" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A33" s="7"/>
       <c r="B33" s="7"/>
       <c r="C33" s="7"/>
@@ -1829,7 +1845,7 @@
       <c r="W33" s="7"/>
       <c r="X33" s="7"/>
     </row>
-    <row r="34" spans="1:24" ht="12">
+    <row r="34" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A34" s="7"/>
       <c r="B34" s="7"/>
       <c r="C34" s="7"/>
@@ -1855,7 +1871,7 @@
       <c r="W34" s="7"/>
       <c r="X34" s="7"/>
     </row>
-    <row r="35" spans="1:24" ht="12">
+    <row r="35" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A35" s="7"/>
       <c r="B35" s="7"/>
       <c r="C35" s="7"/>
@@ -1881,2866 +1897,2866 @@
       <c r="W35" s="7"/>
       <c r="X35" s="7"/>
     </row>
-    <row r="36" spans="1:24" ht="12">
+    <row r="36" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B36" s="6"/>
     </row>
-    <row r="37" spans="1:24" ht="12">
+    <row r="37" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B37" s="6"/>
     </row>
-    <row r="38" spans="1:24" ht="12">
+    <row r="38" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B38" s="6"/>
     </row>
-    <row r="39" spans="1:24" ht="12">
+    <row r="39" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B39" s="6"/>
     </row>
-    <row r="40" spans="1:24" ht="12">
+    <row r="40" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B40" s="6"/>
     </row>
-    <row r="41" spans="1:24" ht="12">
+    <row r="41" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B41" s="6"/>
     </row>
-    <row r="42" spans="1:24" ht="12">
+    <row r="42" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B42" s="6"/>
     </row>
-    <row r="43" spans="1:24" ht="12">
+    <row r="43" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B43" s="6"/>
     </row>
-    <row r="44" spans="1:24" ht="12">
+    <row r="44" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B44" s="6"/>
     </row>
-    <row r="45" spans="1:24" ht="12">
+    <row r="45" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B45" s="6"/>
     </row>
-    <row r="46" spans="1:24" ht="12">
+    <row r="46" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B46" s="6"/>
     </row>
-    <row r="47" spans="1:24" ht="12">
+    <row r="47" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B47" s="6"/>
     </row>
-    <row r="48" spans="1:24" ht="12">
+    <row r="48" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B48" s="6"/>
     </row>
-    <row r="49" spans="2:2" ht="12">
+    <row r="49" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B49" s="6"/>
     </row>
-    <row r="50" spans="2:2" ht="12">
+    <row r="50" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B50" s="6"/>
     </row>
-    <row r="51" spans="2:2" ht="12">
+    <row r="51" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B51" s="6"/>
     </row>
-    <row r="52" spans="2:2" ht="12">
+    <row r="52" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B52" s="6"/>
     </row>
-    <row r="53" spans="2:2" ht="12">
+    <row r="53" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B53" s="6"/>
     </row>
-    <row r="54" spans="2:2" ht="12">
+    <row r="54" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B54" s="6"/>
     </row>
-    <row r="55" spans="2:2" ht="12">
+    <row r="55" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B55" s="6"/>
     </row>
-    <row r="56" spans="2:2" ht="12">
+    <row r="56" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B56" s="6"/>
     </row>
-    <row r="57" spans="2:2" ht="12">
+    <row r="57" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B57" s="6"/>
     </row>
-    <row r="58" spans="2:2" ht="12">
+    <row r="58" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B58" s="6"/>
     </row>
-    <row r="59" spans="2:2" ht="12">
+    <row r="59" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B59" s="6"/>
     </row>
-    <row r="60" spans="2:2" ht="12">
+    <row r="60" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B60" s="6"/>
     </row>
-    <row r="61" spans="2:2" ht="12">
+    <row r="61" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B61" s="6"/>
     </row>
-    <row r="62" spans="2:2" ht="12">
+    <row r="62" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B62" s="6"/>
     </row>
-    <row r="63" spans="2:2" ht="12">
+    <row r="63" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B63" s="6"/>
     </row>
-    <row r="64" spans="2:2" ht="12">
+    <row r="64" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B64" s="6"/>
     </row>
-    <row r="65" spans="2:2" ht="12">
+    <row r="65" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B65" s="6"/>
     </row>
-    <row r="66" spans="2:2" ht="12">
+    <row r="66" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B66" s="6"/>
     </row>
-    <row r="67" spans="2:2" ht="12">
+    <row r="67" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B67" s="6"/>
     </row>
-    <row r="68" spans="2:2" ht="12">
+    <row r="68" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B68" s="6"/>
     </row>
-    <row r="69" spans="2:2" ht="12">
+    <row r="69" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B69" s="6"/>
     </row>
-    <row r="70" spans="2:2" ht="12">
+    <row r="70" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B70" s="6"/>
     </row>
-    <row r="71" spans="2:2" ht="12">
+    <row r="71" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B71" s="6"/>
     </row>
-    <row r="72" spans="2:2" ht="12">
+    <row r="72" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B72" s="6"/>
     </row>
-    <row r="73" spans="2:2" ht="12">
+    <row r="73" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B73" s="6"/>
     </row>
-    <row r="74" spans="2:2" ht="12">
+    <row r="74" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B74" s="6"/>
     </row>
-    <row r="75" spans="2:2" ht="12">
+    <row r="75" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B75" s="6"/>
     </row>
-    <row r="76" spans="2:2" ht="12">
+    <row r="76" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B76" s="6"/>
     </row>
-    <row r="77" spans="2:2" ht="12">
+    <row r="77" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B77" s="6"/>
     </row>
-    <row r="78" spans="2:2" ht="12">
+    <row r="78" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B78" s="6"/>
     </row>
-    <row r="79" spans="2:2" ht="12">
+    <row r="79" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B79" s="6"/>
     </row>
-    <row r="80" spans="2:2" ht="12">
+    <row r="80" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B80" s="6"/>
     </row>
-    <row r="81" spans="2:2" ht="12">
+    <row r="81" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B81" s="6"/>
     </row>
-    <row r="82" spans="2:2" ht="12">
+    <row r="82" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B82" s="6"/>
     </row>
-    <row r="83" spans="2:2" ht="12">
+    <row r="83" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B83" s="6"/>
     </row>
-    <row r="84" spans="2:2" ht="12">
+    <row r="84" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B84" s="6"/>
     </row>
-    <row r="85" spans="2:2" ht="12">
+    <row r="85" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B85" s="6"/>
     </row>
-    <row r="86" spans="2:2" ht="12">
+    <row r="86" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B86" s="6"/>
     </row>
-    <row r="87" spans="2:2" ht="12">
+    <row r="87" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B87" s="6"/>
     </row>
-    <row r="88" spans="2:2" ht="12">
+    <row r="88" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B88" s="6"/>
     </row>
-    <row r="89" spans="2:2" ht="12">
+    <row r="89" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B89" s="6"/>
     </row>
-    <row r="90" spans="2:2" ht="12">
+    <row r="90" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B90" s="6"/>
     </row>
-    <row r="91" spans="2:2" ht="12">
+    <row r="91" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B91" s="6"/>
     </row>
-    <row r="92" spans="2:2" ht="12">
+    <row r="92" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B92" s="6"/>
     </row>
-    <row r="93" spans="2:2" ht="12">
+    <row r="93" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B93" s="6"/>
     </row>
-    <row r="94" spans="2:2" ht="12">
+    <row r="94" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B94" s="6"/>
     </row>
-    <row r="95" spans="2:2" ht="12">
+    <row r="95" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B95" s="6"/>
     </row>
-    <row r="96" spans="2:2" ht="12">
+    <row r="96" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B96" s="6"/>
     </row>
-    <row r="97" spans="2:2" ht="12">
+    <row r="97" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B97" s="6"/>
     </row>
-    <row r="98" spans="2:2" ht="12">
+    <row r="98" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B98" s="6"/>
     </row>
-    <row r="99" spans="2:2" ht="12">
+    <row r="99" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B99" s="6"/>
     </row>
-    <row r="100" spans="2:2" ht="12">
+    <row r="100" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B100" s="6"/>
     </row>
-    <row r="101" spans="2:2" ht="12">
+    <row r="101" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B101" s="6"/>
     </row>
-    <row r="102" spans="2:2" ht="12">
+    <row r="102" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B102" s="6"/>
     </row>
-    <row r="103" spans="2:2" ht="12">
+    <row r="103" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B103" s="6"/>
     </row>
-    <row r="104" spans="2:2" ht="12">
+    <row r="104" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B104" s="6"/>
     </row>
-    <row r="105" spans="2:2" ht="12">
+    <row r="105" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B105" s="6"/>
     </row>
-    <row r="106" spans="2:2" ht="12">
+    <row r="106" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B106" s="6"/>
     </row>
-    <row r="107" spans="2:2" ht="12">
+    <row r="107" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B107" s="6"/>
     </row>
-    <row r="108" spans="2:2" ht="12">
+    <row r="108" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B108" s="6"/>
     </row>
-    <row r="109" spans="2:2" ht="12">
+    <row r="109" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B109" s="6"/>
     </row>
-    <row r="110" spans="2:2" ht="12">
+    <row r="110" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B110" s="6"/>
     </row>
-    <row r="111" spans="2:2" ht="12">
+    <row r="111" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B111" s="6"/>
     </row>
-    <row r="112" spans="2:2" ht="12">
+    <row r="112" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B112" s="6"/>
     </row>
-    <row r="113" spans="2:2" ht="12">
+    <row r="113" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B113" s="6"/>
     </row>
-    <row r="114" spans="2:2" ht="12">
+    <row r="114" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B114" s="6"/>
     </row>
-    <row r="115" spans="2:2" ht="12">
+    <row r="115" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B115" s="6"/>
     </row>
-    <row r="116" spans="2:2" ht="12">
+    <row r="116" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B116" s="6"/>
     </row>
-    <row r="117" spans="2:2" ht="12">
+    <row r="117" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B117" s="6"/>
     </row>
-    <row r="118" spans="2:2" ht="12">
+    <row r="118" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B118" s="6"/>
     </row>
-    <row r="119" spans="2:2" ht="12">
+    <row r="119" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B119" s="6"/>
     </row>
-    <row r="120" spans="2:2" ht="12">
+    <row r="120" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B120" s="6"/>
     </row>
-    <row r="121" spans="2:2" ht="12">
+    <row r="121" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B121" s="6"/>
     </row>
-    <row r="122" spans="2:2" ht="12">
+    <row r="122" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B122" s="6"/>
     </row>
-    <row r="123" spans="2:2" ht="12">
+    <row r="123" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B123" s="6"/>
     </row>
-    <row r="124" spans="2:2" ht="12">
+    <row r="124" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B124" s="6"/>
     </row>
-    <row r="125" spans="2:2" ht="12">
+    <row r="125" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B125" s="6"/>
     </row>
-    <row r="126" spans="2:2" ht="12">
+    <row r="126" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B126" s="6"/>
     </row>
-    <row r="127" spans="2:2" ht="12">
+    <row r="127" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B127" s="6"/>
     </row>
-    <row r="128" spans="2:2" ht="12">
+    <row r="128" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B128" s="6"/>
     </row>
-    <row r="129" spans="2:2" ht="12">
+    <row r="129" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B129" s="6"/>
     </row>
-    <row r="130" spans="2:2" ht="12">
+    <row r="130" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B130" s="6"/>
     </row>
-    <row r="131" spans="2:2" ht="12">
+    <row r="131" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B131" s="6"/>
     </row>
-    <row r="132" spans="2:2" ht="12">
+    <row r="132" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B132" s="6"/>
     </row>
-    <row r="133" spans="2:2" ht="12">
+    <row r="133" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B133" s="6"/>
     </row>
-    <row r="134" spans="2:2" ht="12">
+    <row r="134" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B134" s="6"/>
     </row>
-    <row r="135" spans="2:2" ht="12">
+    <row r="135" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B135" s="6"/>
     </row>
-    <row r="136" spans="2:2" ht="12">
+    <row r="136" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B136" s="6"/>
     </row>
-    <row r="137" spans="2:2" ht="12">
+    <row r="137" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B137" s="6"/>
     </row>
-    <row r="138" spans="2:2" ht="12">
+    <row r="138" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B138" s="6"/>
     </row>
-    <row r="139" spans="2:2" ht="12">
+    <row r="139" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B139" s="6"/>
     </row>
-    <row r="140" spans="2:2" ht="12">
+    <row r="140" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B140" s="6"/>
     </row>
-    <row r="141" spans="2:2" ht="12">
+    <row r="141" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B141" s="6"/>
     </row>
-    <row r="142" spans="2:2" ht="12">
+    <row r="142" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B142" s="6"/>
     </row>
-    <row r="143" spans="2:2" ht="12">
+    <row r="143" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B143" s="6"/>
     </row>
-    <row r="144" spans="2:2" ht="12">
+    <row r="144" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B144" s="6"/>
     </row>
-    <row r="145" spans="2:2" ht="12">
+    <row r="145" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B145" s="6"/>
     </row>
-    <row r="146" spans="2:2" ht="12">
+    <row r="146" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B146" s="6"/>
     </row>
-    <row r="147" spans="2:2" ht="12">
+    <row r="147" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B147" s="6"/>
     </row>
-    <row r="148" spans="2:2" ht="12">
+    <row r="148" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B148" s="6"/>
     </row>
-    <row r="149" spans="2:2" ht="12">
+    <row r="149" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B149" s="6"/>
     </row>
-    <row r="150" spans="2:2" ht="12">
+    <row r="150" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B150" s="6"/>
     </row>
-    <row r="151" spans="2:2" ht="12">
+    <row r="151" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B151" s="6"/>
     </row>
-    <row r="152" spans="2:2" ht="12">
+    <row r="152" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B152" s="6"/>
     </row>
-    <row r="153" spans="2:2" ht="12">
+    <row r="153" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B153" s="6"/>
     </row>
-    <row r="154" spans="2:2" ht="12">
+    <row r="154" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B154" s="6"/>
     </row>
-    <row r="155" spans="2:2" ht="12">
+    <row r="155" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B155" s="6"/>
     </row>
-    <row r="156" spans="2:2" ht="12">
+    <row r="156" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B156" s="6"/>
     </row>
-    <row r="157" spans="2:2" ht="12">
+    <row r="157" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B157" s="6"/>
     </row>
-    <row r="158" spans="2:2" ht="12">
+    <row r="158" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B158" s="6"/>
     </row>
-    <row r="159" spans="2:2" ht="12">
+    <row r="159" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B159" s="6"/>
     </row>
-    <row r="160" spans="2:2" ht="12">
+    <row r="160" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B160" s="6"/>
     </row>
-    <row r="161" spans="2:2" ht="12">
+    <row r="161" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B161" s="6"/>
     </row>
-    <row r="162" spans="2:2" ht="12">
+    <row r="162" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B162" s="6"/>
     </row>
-    <row r="163" spans="2:2" ht="12">
+    <row r="163" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B163" s="6"/>
     </row>
-    <row r="164" spans="2:2" ht="12">
+    <row r="164" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B164" s="6"/>
     </row>
-    <row r="165" spans="2:2" ht="12">
+    <row r="165" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B165" s="6"/>
     </row>
-    <row r="166" spans="2:2" ht="12">
+    <row r="166" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B166" s="6"/>
     </row>
-    <row r="167" spans="2:2" ht="12">
+    <row r="167" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B167" s="6"/>
     </row>
-    <row r="168" spans="2:2" ht="12">
+    <row r="168" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B168" s="6"/>
     </row>
-    <row r="169" spans="2:2" ht="12">
+    <row r="169" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B169" s="6"/>
     </row>
-    <row r="170" spans="2:2" ht="12">
+    <row r="170" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B170" s="6"/>
     </row>
-    <row r="171" spans="2:2" ht="12">
+    <row r="171" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B171" s="6"/>
     </row>
-    <row r="172" spans="2:2" ht="12">
+    <row r="172" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B172" s="6"/>
     </row>
-    <row r="173" spans="2:2" ht="12">
+    <row r="173" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B173" s="6"/>
     </row>
-    <row r="174" spans="2:2" ht="12">
+    <row r="174" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B174" s="6"/>
     </row>
-    <row r="175" spans="2:2" ht="12">
+    <row r="175" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B175" s="6"/>
     </row>
-    <row r="176" spans="2:2" ht="12">
+    <row r="176" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B176" s="6"/>
     </row>
-    <row r="177" spans="2:2" ht="12">
+    <row r="177" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B177" s="6"/>
     </row>
-    <row r="178" spans="2:2" ht="12">
+    <row r="178" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B178" s="6"/>
     </row>
-    <row r="179" spans="2:2" ht="12">
+    <row r="179" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B179" s="6"/>
     </row>
-    <row r="180" spans="2:2" ht="12">
+    <row r="180" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B180" s="6"/>
     </row>
-    <row r="181" spans="2:2" ht="12">
+    <row r="181" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B181" s="6"/>
     </row>
-    <row r="182" spans="2:2" ht="12">
+    <row r="182" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B182" s="6"/>
     </row>
-    <row r="183" spans="2:2" ht="12">
+    <row r="183" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B183" s="6"/>
     </row>
-    <row r="184" spans="2:2" ht="12">
+    <row r="184" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B184" s="6"/>
     </row>
-    <row r="185" spans="2:2" ht="12">
+    <row r="185" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B185" s="6"/>
     </row>
-    <row r="186" spans="2:2" ht="12">
+    <row r="186" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B186" s="6"/>
     </row>
-    <row r="187" spans="2:2" ht="12">
+    <row r="187" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B187" s="6"/>
     </row>
-    <row r="188" spans="2:2" ht="12">
+    <row r="188" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B188" s="6"/>
     </row>
-    <row r="189" spans="2:2" ht="12">
+    <row r="189" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B189" s="6"/>
     </row>
-    <row r="190" spans="2:2" ht="12">
+    <row r="190" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B190" s="6"/>
     </row>
-    <row r="191" spans="2:2" ht="12">
+    <row r="191" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B191" s="6"/>
     </row>
-    <row r="192" spans="2:2" ht="12">
+    <row r="192" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B192" s="6"/>
     </row>
-    <row r="193" spans="2:2" ht="12">
+    <row r="193" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B193" s="6"/>
     </row>
-    <row r="194" spans="2:2" ht="12">
+    <row r="194" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B194" s="6"/>
     </row>
-    <row r="195" spans="2:2" ht="12">
+    <row r="195" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B195" s="6"/>
     </row>
-    <row r="196" spans="2:2" ht="12">
+    <row r="196" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B196" s="6"/>
     </row>
-    <row r="197" spans="2:2" ht="12">
+    <row r="197" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B197" s="6"/>
     </row>
-    <row r="198" spans="2:2" ht="12">
+    <row r="198" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B198" s="6"/>
     </row>
-    <row r="199" spans="2:2" ht="12">
+    <row r="199" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B199" s="6"/>
     </row>
-    <row r="200" spans="2:2" ht="12">
+    <row r="200" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B200" s="6"/>
     </row>
-    <row r="201" spans="2:2" ht="12">
+    <row r="201" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B201" s="6"/>
     </row>
-    <row r="202" spans="2:2" ht="12">
+    <row r="202" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B202" s="6"/>
     </row>
-    <row r="203" spans="2:2" ht="12">
+    <row r="203" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B203" s="6"/>
     </row>
-    <row r="204" spans="2:2" ht="12">
+    <row r="204" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B204" s="6"/>
     </row>
-    <row r="205" spans="2:2" ht="12">
+    <row r="205" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B205" s="6"/>
     </row>
-    <row r="206" spans="2:2" ht="12">
+    <row r="206" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B206" s="6"/>
     </row>
-    <row r="207" spans="2:2" ht="12">
+    <row r="207" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B207" s="6"/>
     </row>
-    <row r="208" spans="2:2" ht="12">
+    <row r="208" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B208" s="6"/>
     </row>
-    <row r="209" spans="2:2" ht="12">
+    <row r="209" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B209" s="6"/>
     </row>
-    <row r="210" spans="2:2" ht="12">
+    <row r="210" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B210" s="6"/>
     </row>
-    <row r="211" spans="2:2" ht="12">
+    <row r="211" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B211" s="6"/>
     </row>
-    <row r="212" spans="2:2" ht="12">
+    <row r="212" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B212" s="6"/>
     </row>
-    <row r="213" spans="2:2" ht="12">
+    <row r="213" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B213" s="6"/>
     </row>
-    <row r="214" spans="2:2" ht="12">
+    <row r="214" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B214" s="6"/>
     </row>
-    <row r="215" spans="2:2" ht="12">
+    <row r="215" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B215" s="6"/>
     </row>
-    <row r="216" spans="2:2" ht="12">
+    <row r="216" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B216" s="6"/>
     </row>
-    <row r="217" spans="2:2" ht="12">
+    <row r="217" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B217" s="6"/>
     </row>
-    <row r="218" spans="2:2" ht="12">
+    <row r="218" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B218" s="6"/>
     </row>
-    <row r="219" spans="2:2" ht="12">
+    <row r="219" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B219" s="6"/>
     </row>
-    <row r="220" spans="2:2" ht="12">
+    <row r="220" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B220" s="6"/>
     </row>
-    <row r="221" spans="2:2" ht="12">
+    <row r="221" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B221" s="6"/>
     </row>
-    <row r="222" spans="2:2" ht="12">
+    <row r="222" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B222" s="6"/>
     </row>
-    <row r="223" spans="2:2" ht="12">
+    <row r="223" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B223" s="6"/>
     </row>
-    <row r="224" spans="2:2" ht="12">
+    <row r="224" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B224" s="6"/>
     </row>
-    <row r="225" spans="2:2" ht="12">
+    <row r="225" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B225" s="6"/>
     </row>
-    <row r="226" spans="2:2" ht="12">
+    <row r="226" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B226" s="6"/>
     </row>
-    <row r="227" spans="2:2" ht="12">
+    <row r="227" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B227" s="6"/>
     </row>
-    <row r="228" spans="2:2" ht="12">
+    <row r="228" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B228" s="6"/>
     </row>
-    <row r="229" spans="2:2" ht="12">
+    <row r="229" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B229" s="6"/>
     </row>
-    <row r="230" spans="2:2" ht="12">
+    <row r="230" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B230" s="6"/>
     </row>
-    <row r="231" spans="2:2" ht="12">
+    <row r="231" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B231" s="6"/>
     </row>
-    <row r="232" spans="2:2" ht="12">
+    <row r="232" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B232" s="6"/>
     </row>
-    <row r="233" spans="2:2" ht="12">
+    <row r="233" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B233" s="6"/>
     </row>
-    <row r="234" spans="2:2" ht="12">
+    <row r="234" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B234" s="6"/>
     </row>
-    <row r="235" spans="2:2" ht="12">
+    <row r="235" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B235" s="6"/>
     </row>
-    <row r="236" spans="2:2" ht="12">
+    <row r="236" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B236" s="6"/>
     </row>
-    <row r="237" spans="2:2" ht="12">
+    <row r="237" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B237" s="6"/>
     </row>
-    <row r="238" spans="2:2" ht="12">
+    <row r="238" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B238" s="6"/>
     </row>
-    <row r="239" spans="2:2" ht="12">
+    <row r="239" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B239" s="6"/>
     </row>
-    <row r="240" spans="2:2" ht="12">
+    <row r="240" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B240" s="6"/>
     </row>
-    <row r="241" spans="2:2" ht="12">
+    <row r="241" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B241" s="6"/>
     </row>
-    <row r="242" spans="2:2" ht="12">
+    <row r="242" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B242" s="6"/>
     </row>
-    <row r="243" spans="2:2" ht="12">
+    <row r="243" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B243" s="6"/>
     </row>
-    <row r="244" spans="2:2" ht="12">
+    <row r="244" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B244" s="6"/>
     </row>
-    <row r="245" spans="2:2" ht="12">
+    <row r="245" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B245" s="6"/>
     </row>
-    <row r="246" spans="2:2" ht="12">
+    <row r="246" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B246" s="6"/>
     </row>
-    <row r="247" spans="2:2" ht="12">
+    <row r="247" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B247" s="6"/>
     </row>
-    <row r="248" spans="2:2" ht="12">
+    <row r="248" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B248" s="6"/>
     </row>
-    <row r="249" spans="2:2" ht="12">
+    <row r="249" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B249" s="6"/>
     </row>
-    <row r="250" spans="2:2" ht="12">
+    <row r="250" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B250" s="6"/>
     </row>
-    <row r="251" spans="2:2" ht="12">
+    <row r="251" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B251" s="6"/>
     </row>
-    <row r="252" spans="2:2" ht="12">
+    <row r="252" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B252" s="6"/>
     </row>
-    <row r="253" spans="2:2" ht="12">
+    <row r="253" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B253" s="6"/>
     </row>
-    <row r="254" spans="2:2" ht="12">
+    <row r="254" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B254" s="6"/>
     </row>
-    <row r="255" spans="2:2" ht="12">
+    <row r="255" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B255" s="6"/>
     </row>
-    <row r="256" spans="2:2" ht="12">
+    <row r="256" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B256" s="6"/>
     </row>
-    <row r="257" spans="2:2" ht="12">
+    <row r="257" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B257" s="6"/>
     </row>
-    <row r="258" spans="2:2" ht="12">
+    <row r="258" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B258" s="6"/>
     </row>
-    <row r="259" spans="2:2" ht="12">
+    <row r="259" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B259" s="6"/>
     </row>
-    <row r="260" spans="2:2" ht="12">
+    <row r="260" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B260" s="6"/>
     </row>
-    <row r="261" spans="2:2" ht="12">
+    <row r="261" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B261" s="6"/>
     </row>
-    <row r="262" spans="2:2" ht="12">
+    <row r="262" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B262" s="6"/>
     </row>
-    <row r="263" spans="2:2" ht="12">
+    <row r="263" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B263" s="6"/>
     </row>
-    <row r="264" spans="2:2" ht="12">
+    <row r="264" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B264" s="6"/>
     </row>
-    <row r="265" spans="2:2" ht="12">
+    <row r="265" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B265" s="6"/>
     </row>
-    <row r="266" spans="2:2" ht="12">
+    <row r="266" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B266" s="6"/>
     </row>
-    <row r="267" spans="2:2" ht="12">
+    <row r="267" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B267" s="6"/>
     </row>
-    <row r="268" spans="2:2" ht="12">
+    <row r="268" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B268" s="6"/>
     </row>
-    <row r="269" spans="2:2" ht="12">
+    <row r="269" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B269" s="6"/>
     </row>
-    <row r="270" spans="2:2" ht="12">
+    <row r="270" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B270" s="6"/>
     </row>
-    <row r="271" spans="2:2" ht="12">
+    <row r="271" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B271" s="6"/>
     </row>
-    <row r="272" spans="2:2" ht="12">
+    <row r="272" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B272" s="6"/>
     </row>
-    <row r="273" spans="2:2" ht="12">
+    <row r="273" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B273" s="6"/>
     </row>
-    <row r="274" spans="2:2" ht="12">
+    <row r="274" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B274" s="6"/>
     </row>
-    <row r="275" spans="2:2" ht="12">
+    <row r="275" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B275" s="6"/>
     </row>
-    <row r="276" spans="2:2" ht="12">
+    <row r="276" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B276" s="6"/>
     </row>
-    <row r="277" spans="2:2" ht="12">
+    <row r="277" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B277" s="6"/>
     </row>
-    <row r="278" spans="2:2" ht="12">
+    <row r="278" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B278" s="6"/>
     </row>
-    <row r="279" spans="2:2" ht="12">
+    <row r="279" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B279" s="6"/>
     </row>
-    <row r="280" spans="2:2" ht="12">
+    <row r="280" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B280" s="6"/>
     </row>
-    <row r="281" spans="2:2" ht="12">
+    <row r="281" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B281" s="6"/>
     </row>
-    <row r="282" spans="2:2" ht="12">
+    <row r="282" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B282" s="6"/>
     </row>
-    <row r="283" spans="2:2" ht="12">
+    <row r="283" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B283" s="6"/>
     </row>
-    <row r="284" spans="2:2" ht="12">
+    <row r="284" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B284" s="6"/>
     </row>
-    <row r="285" spans="2:2" ht="12">
+    <row r="285" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B285" s="6"/>
     </row>
-    <row r="286" spans="2:2" ht="12">
+    <row r="286" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B286" s="6"/>
     </row>
-    <row r="287" spans="2:2" ht="12">
+    <row r="287" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B287" s="6"/>
     </row>
-    <row r="288" spans="2:2" ht="12">
+    <row r="288" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B288" s="6"/>
     </row>
-    <row r="289" spans="2:2" ht="12">
+    <row r="289" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B289" s="6"/>
     </row>
-    <row r="290" spans="2:2" ht="12">
+    <row r="290" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B290" s="6"/>
     </row>
-    <row r="291" spans="2:2" ht="12">
+    <row r="291" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B291" s="6"/>
     </row>
-    <row r="292" spans="2:2" ht="12">
+    <row r="292" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B292" s="6"/>
     </row>
-    <row r="293" spans="2:2" ht="12">
+    <row r="293" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B293" s="6"/>
     </row>
-    <row r="294" spans="2:2" ht="12">
+    <row r="294" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B294" s="6"/>
     </row>
-    <row r="295" spans="2:2" ht="12">
+    <row r="295" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B295" s="6"/>
     </row>
-    <row r="296" spans="2:2" ht="12">
+    <row r="296" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B296" s="6"/>
     </row>
-    <row r="297" spans="2:2" ht="12">
+    <row r="297" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B297" s="6"/>
     </row>
-    <row r="298" spans="2:2" ht="12">
+    <row r="298" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B298" s="6"/>
     </row>
-    <row r="299" spans="2:2" ht="12">
+    <row r="299" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B299" s="6"/>
     </row>
-    <row r="300" spans="2:2" ht="12">
+    <row r="300" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B300" s="6"/>
     </row>
-    <row r="301" spans="2:2" ht="12">
+    <row r="301" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B301" s="6"/>
     </row>
-    <row r="302" spans="2:2" ht="12">
+    <row r="302" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B302" s="6"/>
     </row>
-    <row r="303" spans="2:2" ht="12">
+    <row r="303" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B303" s="6"/>
     </row>
-    <row r="304" spans="2:2" ht="12">
+    <row r="304" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B304" s="6"/>
     </row>
-    <row r="305" spans="2:2" ht="12">
+    <row r="305" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B305" s="6"/>
     </row>
-    <row r="306" spans="2:2" ht="12">
+    <row r="306" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B306" s="6"/>
     </row>
-    <row r="307" spans="2:2" ht="12">
+    <row r="307" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B307" s="6"/>
     </row>
-    <row r="308" spans="2:2" ht="12">
+    <row r="308" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B308" s="6"/>
     </row>
-    <row r="309" spans="2:2" ht="12">
+    <row r="309" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B309" s="6"/>
     </row>
-    <row r="310" spans="2:2" ht="12">
+    <row r="310" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B310" s="6"/>
     </row>
-    <row r="311" spans="2:2" ht="12">
+    <row r="311" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B311" s="6"/>
     </row>
-    <row r="312" spans="2:2" ht="12">
+    <row r="312" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B312" s="6"/>
     </row>
-    <row r="313" spans="2:2" ht="12">
+    <row r="313" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B313" s="6"/>
     </row>
-    <row r="314" spans="2:2" ht="12">
+    <row r="314" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B314" s="6"/>
     </row>
-    <row r="315" spans="2:2" ht="12">
+    <row r="315" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B315" s="6"/>
     </row>
-    <row r="316" spans="2:2" ht="12">
+    <row r="316" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B316" s="6"/>
     </row>
-    <row r="317" spans="2:2" ht="12">
+    <row r="317" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B317" s="6"/>
     </row>
-    <row r="318" spans="2:2" ht="12">
+    <row r="318" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B318" s="6"/>
     </row>
-    <row r="319" spans="2:2" ht="12">
+    <row r="319" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B319" s="6"/>
     </row>
-    <row r="320" spans="2:2" ht="12">
+    <row r="320" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B320" s="6"/>
     </row>
-    <row r="321" spans="2:2" ht="12">
+    <row r="321" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B321" s="6"/>
     </row>
-    <row r="322" spans="2:2" ht="12">
+    <row r="322" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B322" s="6"/>
     </row>
-    <row r="323" spans="2:2" ht="12">
+    <row r="323" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B323" s="6"/>
     </row>
-    <row r="324" spans="2:2" ht="12">
+    <row r="324" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B324" s="6"/>
     </row>
-    <row r="325" spans="2:2" ht="12">
+    <row r="325" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B325" s="6"/>
     </row>
-    <row r="326" spans="2:2" ht="12">
+    <row r="326" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B326" s="6"/>
     </row>
-    <row r="327" spans="2:2" ht="12">
+    <row r="327" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B327" s="6"/>
     </row>
-    <row r="328" spans="2:2" ht="12">
+    <row r="328" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B328" s="6"/>
     </row>
-    <row r="329" spans="2:2" ht="12">
+    <row r="329" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B329" s="6"/>
     </row>
-    <row r="330" spans="2:2" ht="12">
+    <row r="330" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B330" s="6"/>
     </row>
-    <row r="331" spans="2:2" ht="12">
+    <row r="331" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B331" s="6"/>
     </row>
-    <row r="332" spans="2:2" ht="12">
+    <row r="332" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B332" s="6"/>
     </row>
-    <row r="333" spans="2:2" ht="12">
+    <row r="333" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B333" s="6"/>
     </row>
-    <row r="334" spans="2:2" ht="12">
+    <row r="334" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B334" s="6"/>
     </row>
-    <row r="335" spans="2:2" ht="12">
+    <row r="335" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B335" s="6"/>
     </row>
-    <row r="336" spans="2:2" ht="12">
+    <row r="336" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B336" s="6"/>
     </row>
-    <row r="337" spans="2:2" ht="12">
+    <row r="337" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B337" s="6"/>
     </row>
-    <row r="338" spans="2:2" ht="12">
+    <row r="338" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B338" s="6"/>
     </row>
-    <row r="339" spans="2:2" ht="12">
+    <row r="339" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B339" s="6"/>
     </row>
-    <row r="340" spans="2:2" ht="12">
+    <row r="340" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B340" s="6"/>
     </row>
-    <row r="341" spans="2:2" ht="12">
+    <row r="341" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B341" s="6"/>
     </row>
-    <row r="342" spans="2:2" ht="12">
+    <row r="342" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B342" s="6"/>
     </row>
-    <row r="343" spans="2:2" ht="12">
+    <row r="343" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B343" s="6"/>
     </row>
-    <row r="344" spans="2:2" ht="12">
+    <row r="344" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B344" s="6"/>
     </row>
-    <row r="345" spans="2:2" ht="12">
+    <row r="345" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B345" s="6"/>
     </row>
-    <row r="346" spans="2:2" ht="12">
+    <row r="346" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B346" s="6"/>
     </row>
-    <row r="347" spans="2:2" ht="12">
+    <row r="347" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B347" s="6"/>
     </row>
-    <row r="348" spans="2:2" ht="12">
+    <row r="348" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B348" s="6"/>
     </row>
-    <row r="349" spans="2:2" ht="12">
+    <row r="349" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B349" s="6"/>
     </row>
-    <row r="350" spans="2:2" ht="12">
+    <row r="350" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B350" s="6"/>
     </row>
-    <row r="351" spans="2:2" ht="12">
+    <row r="351" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B351" s="6"/>
     </row>
-    <row r="352" spans="2:2" ht="12">
+    <row r="352" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B352" s="6"/>
     </row>
-    <row r="353" spans="2:2" ht="12">
+    <row r="353" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B353" s="6"/>
     </row>
-    <row r="354" spans="2:2" ht="12">
+    <row r="354" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B354" s="6"/>
     </row>
-    <row r="355" spans="2:2" ht="12">
+    <row r="355" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B355" s="6"/>
     </row>
-    <row r="356" spans="2:2" ht="12">
+    <row r="356" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B356" s="6"/>
     </row>
-    <row r="357" spans="2:2" ht="12">
+    <row r="357" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B357" s="6"/>
     </row>
-    <row r="358" spans="2:2" ht="12">
+    <row r="358" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B358" s="6"/>
     </row>
-    <row r="359" spans="2:2" ht="12">
+    <row r="359" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B359" s="6"/>
     </row>
-    <row r="360" spans="2:2" ht="12">
+    <row r="360" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B360" s="6"/>
     </row>
-    <row r="361" spans="2:2" ht="12">
+    <row r="361" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B361" s="6"/>
     </row>
-    <row r="362" spans="2:2" ht="12">
+    <row r="362" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B362" s="6"/>
     </row>
-    <row r="363" spans="2:2" ht="12">
+    <row r="363" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B363" s="6"/>
     </row>
-    <row r="364" spans="2:2" ht="12">
+    <row r="364" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B364" s="6"/>
     </row>
-    <row r="365" spans="2:2" ht="12">
+    <row r="365" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B365" s="6"/>
     </row>
-    <row r="366" spans="2:2" ht="12">
+    <row r="366" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B366" s="6"/>
     </row>
-    <row r="367" spans="2:2" ht="12">
+    <row r="367" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B367" s="6"/>
     </row>
-    <row r="368" spans="2:2" ht="12">
+    <row r="368" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B368" s="6"/>
     </row>
-    <row r="369" spans="2:2" ht="12">
+    <row r="369" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B369" s="6"/>
     </row>
-    <row r="370" spans="2:2" ht="12">
+    <row r="370" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B370" s="6"/>
     </row>
-    <row r="371" spans="2:2" ht="12">
+    <row r="371" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B371" s="6"/>
     </row>
-    <row r="372" spans="2:2" ht="12">
+    <row r="372" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B372" s="6"/>
     </row>
-    <row r="373" spans="2:2" ht="12">
+    <row r="373" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B373" s="6"/>
     </row>
-    <row r="374" spans="2:2" ht="12">
+    <row r="374" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B374" s="6"/>
     </row>
-    <row r="375" spans="2:2" ht="12">
+    <row r="375" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B375" s="6"/>
     </row>
-    <row r="376" spans="2:2" ht="12">
+    <row r="376" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B376" s="6"/>
     </row>
-    <row r="377" spans="2:2" ht="12">
+    <row r="377" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B377" s="6"/>
     </row>
-    <row r="378" spans="2:2" ht="12">
+    <row r="378" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B378" s="6"/>
     </row>
-    <row r="379" spans="2:2" ht="12">
+    <row r="379" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B379" s="6"/>
     </row>
-    <row r="380" spans="2:2" ht="12">
+    <row r="380" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B380" s="6"/>
     </row>
-    <row r="381" spans="2:2" ht="12">
+    <row r="381" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B381" s="6"/>
     </row>
-    <row r="382" spans="2:2" ht="12">
+    <row r="382" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B382" s="6"/>
     </row>
-    <row r="383" spans="2:2" ht="12">
+    <row r="383" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B383" s="6"/>
     </row>
-    <row r="384" spans="2:2" ht="12">
+    <row r="384" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B384" s="6"/>
     </row>
-    <row r="385" spans="2:2" ht="12">
+    <row r="385" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B385" s="6"/>
     </row>
-    <row r="386" spans="2:2" ht="12">
+    <row r="386" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B386" s="6"/>
     </row>
-    <row r="387" spans="2:2" ht="12">
+    <row r="387" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B387" s="6"/>
     </row>
-    <row r="388" spans="2:2" ht="12">
+    <row r="388" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B388" s="6"/>
     </row>
-    <row r="389" spans="2:2" ht="12">
+    <row r="389" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B389" s="6"/>
     </row>
-    <row r="390" spans="2:2" ht="12">
+    <row r="390" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B390" s="6"/>
     </row>
-    <row r="391" spans="2:2" ht="12">
+    <row r="391" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B391" s="6"/>
     </row>
-    <row r="392" spans="2:2" ht="12">
+    <row r="392" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B392" s="6"/>
     </row>
-    <row r="393" spans="2:2" ht="12">
+    <row r="393" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B393" s="6"/>
     </row>
-    <row r="394" spans="2:2" ht="12">
+    <row r="394" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B394" s="6"/>
     </row>
-    <row r="395" spans="2:2" ht="12">
+    <row r="395" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B395" s="6"/>
     </row>
-    <row r="396" spans="2:2" ht="12">
+    <row r="396" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B396" s="6"/>
     </row>
-    <row r="397" spans="2:2" ht="12">
+    <row r="397" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B397" s="6"/>
     </row>
-    <row r="398" spans="2:2" ht="12">
+    <row r="398" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B398" s="6"/>
     </row>
-    <row r="399" spans="2:2" ht="12">
+    <row r="399" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B399" s="6"/>
     </row>
-    <row r="400" spans="2:2" ht="12">
+    <row r="400" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B400" s="6"/>
     </row>
-    <row r="401" spans="2:2" ht="12">
+    <row r="401" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B401" s="6"/>
     </row>
-    <row r="402" spans="2:2" ht="12">
+    <row r="402" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B402" s="6"/>
     </row>
-    <row r="403" spans="2:2" ht="12">
+    <row r="403" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B403" s="6"/>
     </row>
-    <row r="404" spans="2:2" ht="12">
+    <row r="404" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B404" s="6"/>
     </row>
-    <row r="405" spans="2:2" ht="12">
+    <row r="405" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B405" s="6"/>
     </row>
-    <row r="406" spans="2:2" ht="12">
+    <row r="406" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B406" s="6"/>
     </row>
-    <row r="407" spans="2:2" ht="12">
+    <row r="407" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B407" s="6"/>
     </row>
-    <row r="408" spans="2:2" ht="12">
+    <row r="408" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B408" s="6"/>
     </row>
-    <row r="409" spans="2:2" ht="12">
+    <row r="409" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B409" s="6"/>
     </row>
-    <row r="410" spans="2:2" ht="12">
+    <row r="410" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B410" s="6"/>
     </row>
-    <row r="411" spans="2:2" ht="12">
+    <row r="411" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B411" s="6"/>
     </row>
-    <row r="412" spans="2:2" ht="12">
+    <row r="412" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B412" s="6"/>
     </row>
-    <row r="413" spans="2:2" ht="12">
+    <row r="413" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B413" s="6"/>
     </row>
-    <row r="414" spans="2:2" ht="12">
+    <row r="414" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B414" s="6"/>
     </row>
-    <row r="415" spans="2:2" ht="12">
+    <row r="415" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B415" s="6"/>
     </row>
-    <row r="416" spans="2:2" ht="12">
+    <row r="416" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B416" s="6"/>
     </row>
-    <row r="417" spans="2:2" ht="12">
+    <row r="417" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B417" s="6"/>
     </row>
-    <row r="418" spans="2:2" ht="12">
+    <row r="418" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B418" s="6"/>
     </row>
-    <row r="419" spans="2:2" ht="12">
+    <row r="419" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B419" s="6"/>
     </row>
-    <row r="420" spans="2:2" ht="12">
+    <row r="420" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B420" s="6"/>
     </row>
-    <row r="421" spans="2:2" ht="12">
+    <row r="421" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B421" s="6"/>
     </row>
-    <row r="422" spans="2:2" ht="12">
+    <row r="422" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B422" s="6"/>
     </row>
-    <row r="423" spans="2:2" ht="12">
+    <row r="423" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B423" s="6"/>
     </row>
-    <row r="424" spans="2:2" ht="12">
+    <row r="424" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B424" s="6"/>
     </row>
-    <row r="425" spans="2:2" ht="12">
+    <row r="425" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B425" s="6"/>
     </row>
-    <row r="426" spans="2:2" ht="12">
+    <row r="426" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B426" s="6"/>
     </row>
-    <row r="427" spans="2:2" ht="12">
+    <row r="427" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B427" s="6"/>
     </row>
-    <row r="428" spans="2:2" ht="12">
+    <row r="428" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B428" s="6"/>
     </row>
-    <row r="429" spans="2:2" ht="12">
+    <row r="429" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B429" s="6"/>
     </row>
-    <row r="430" spans="2:2" ht="12">
+    <row r="430" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B430" s="6"/>
     </row>
-    <row r="431" spans="2:2" ht="12">
+    <row r="431" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B431" s="6"/>
     </row>
-    <row r="432" spans="2:2" ht="12">
+    <row r="432" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B432" s="6"/>
     </row>
-    <row r="433" spans="2:2" ht="12">
+    <row r="433" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B433" s="6"/>
     </row>
-    <row r="434" spans="2:2" ht="12">
+    <row r="434" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B434" s="6"/>
     </row>
-    <row r="435" spans="2:2" ht="12">
+    <row r="435" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B435" s="6"/>
     </row>
-    <row r="436" spans="2:2" ht="12">
+    <row r="436" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B436" s="6"/>
     </row>
-    <row r="437" spans="2:2" ht="12">
+    <row r="437" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B437" s="6"/>
     </row>
-    <row r="438" spans="2:2" ht="12">
+    <row r="438" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B438" s="6"/>
     </row>
-    <row r="439" spans="2:2" ht="12">
+    <row r="439" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B439" s="6"/>
     </row>
-    <row r="440" spans="2:2" ht="12">
+    <row r="440" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B440" s="6"/>
     </row>
-    <row r="441" spans="2:2" ht="12">
+    <row r="441" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B441" s="6"/>
     </row>
-    <row r="442" spans="2:2" ht="12">
+    <row r="442" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B442" s="6"/>
     </row>
-    <row r="443" spans="2:2" ht="12">
+    <row r="443" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B443" s="6"/>
     </row>
-    <row r="444" spans="2:2" ht="12">
+    <row r="444" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B444" s="6"/>
     </row>
-    <row r="445" spans="2:2" ht="12">
+    <row r="445" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B445" s="6"/>
     </row>
-    <row r="446" spans="2:2" ht="12">
+    <row r="446" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B446" s="6"/>
     </row>
-    <row r="447" spans="2:2" ht="12">
+    <row r="447" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B447" s="6"/>
     </row>
-    <row r="448" spans="2:2" ht="12">
+    <row r="448" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B448" s="6"/>
     </row>
-    <row r="449" spans="2:2" ht="12">
+    <row r="449" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B449" s="6"/>
     </row>
-    <row r="450" spans="2:2" ht="12">
+    <row r="450" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B450" s="6"/>
     </row>
-    <row r="451" spans="2:2" ht="12">
+    <row r="451" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B451" s="6"/>
     </row>
-    <row r="452" spans="2:2" ht="12">
+    <row r="452" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B452" s="6"/>
     </row>
-    <row r="453" spans="2:2" ht="12">
+    <row r="453" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B453" s="6"/>
     </row>
-    <row r="454" spans="2:2" ht="12">
+    <row r="454" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B454" s="6"/>
     </row>
-    <row r="455" spans="2:2" ht="12">
+    <row r="455" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B455" s="6"/>
     </row>
-    <row r="456" spans="2:2" ht="12">
+    <row r="456" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B456" s="6"/>
     </row>
-    <row r="457" spans="2:2" ht="12">
+    <row r="457" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B457" s="6"/>
     </row>
-    <row r="458" spans="2:2" ht="12">
+    <row r="458" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B458" s="6"/>
     </row>
-    <row r="459" spans="2:2" ht="12">
+    <row r="459" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B459" s="6"/>
     </row>
-    <row r="460" spans="2:2" ht="12">
+    <row r="460" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B460" s="6"/>
     </row>
-    <row r="461" spans="2:2" ht="12">
+    <row r="461" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B461" s="6"/>
     </row>
-    <row r="462" spans="2:2" ht="12">
+    <row r="462" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B462" s="6"/>
     </row>
-    <row r="463" spans="2:2" ht="12">
+    <row r="463" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B463" s="6"/>
     </row>
-    <row r="464" spans="2:2" ht="12">
+    <row r="464" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B464" s="6"/>
     </row>
-    <row r="465" spans="2:2" ht="12">
+    <row r="465" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B465" s="6"/>
     </row>
-    <row r="466" spans="2:2" ht="12">
+    <row r="466" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B466" s="6"/>
     </row>
-    <row r="467" spans="2:2" ht="12">
+    <row r="467" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B467" s="6"/>
     </row>
-    <row r="468" spans="2:2" ht="12">
+    <row r="468" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B468" s="6"/>
     </row>
-    <row r="469" spans="2:2" ht="12">
+    <row r="469" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B469" s="6"/>
     </row>
-    <row r="470" spans="2:2" ht="12">
+    <row r="470" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B470" s="6"/>
     </row>
-    <row r="471" spans="2:2" ht="12">
+    <row r="471" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B471" s="6"/>
     </row>
-    <row r="472" spans="2:2" ht="12">
+    <row r="472" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B472" s="6"/>
     </row>
-    <row r="473" spans="2:2" ht="12">
+    <row r="473" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B473" s="6"/>
     </row>
-    <row r="474" spans="2:2" ht="12">
+    <row r="474" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B474" s="6"/>
     </row>
-    <row r="475" spans="2:2" ht="12">
+    <row r="475" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B475" s="6"/>
     </row>
-    <row r="476" spans="2:2" ht="12">
+    <row r="476" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B476" s="6"/>
     </row>
-    <row r="477" spans="2:2" ht="12">
+    <row r="477" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B477" s="6"/>
     </row>
-    <row r="478" spans="2:2" ht="12">
+    <row r="478" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B478" s="6"/>
     </row>
-    <row r="479" spans="2:2" ht="12">
+    <row r="479" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B479" s="6"/>
     </row>
-    <row r="480" spans="2:2" ht="12">
+    <row r="480" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B480" s="6"/>
     </row>
-    <row r="481" spans="2:2" ht="12">
+    <row r="481" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B481" s="6"/>
     </row>
-    <row r="482" spans="2:2" ht="12">
+    <row r="482" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B482" s="6"/>
     </row>
-    <row r="483" spans="2:2" ht="12">
+    <row r="483" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B483" s="6"/>
     </row>
-    <row r="484" spans="2:2" ht="12">
+    <row r="484" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B484" s="6"/>
     </row>
-    <row r="485" spans="2:2" ht="12">
+    <row r="485" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B485" s="6"/>
     </row>
-    <row r="486" spans="2:2" ht="12">
+    <row r="486" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B486" s="6"/>
     </row>
-    <row r="487" spans="2:2" ht="12">
+    <row r="487" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B487" s="6"/>
     </row>
-    <row r="488" spans="2:2" ht="12">
+    <row r="488" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B488" s="6"/>
     </row>
-    <row r="489" spans="2:2" ht="12">
+    <row r="489" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B489" s="6"/>
     </row>
-    <row r="490" spans="2:2" ht="12">
+    <row r="490" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B490" s="6"/>
     </row>
-    <row r="491" spans="2:2" ht="12">
+    <row r="491" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B491" s="6"/>
     </row>
-    <row r="492" spans="2:2" ht="12">
+    <row r="492" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B492" s="6"/>
     </row>
-    <row r="493" spans="2:2" ht="12">
+    <row r="493" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B493" s="6"/>
     </row>
-    <row r="494" spans="2:2" ht="12">
+    <row r="494" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B494" s="6"/>
     </row>
-    <row r="495" spans="2:2" ht="12">
+    <row r="495" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B495" s="6"/>
     </row>
-    <row r="496" spans="2:2" ht="12">
+    <row r="496" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B496" s="6"/>
     </row>
-    <row r="497" spans="2:2" ht="12">
+    <row r="497" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B497" s="6"/>
     </row>
-    <row r="498" spans="2:2" ht="12">
+    <row r="498" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B498" s="6"/>
     </row>
-    <row r="499" spans="2:2" ht="12">
+    <row r="499" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B499" s="6"/>
     </row>
-    <row r="500" spans="2:2" ht="12">
+    <row r="500" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B500" s="6"/>
     </row>
-    <row r="501" spans="2:2" ht="12">
+    <row r="501" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B501" s="6"/>
     </row>
-    <row r="502" spans="2:2" ht="12">
+    <row r="502" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B502" s="6"/>
     </row>
-    <row r="503" spans="2:2" ht="12">
+    <row r="503" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B503" s="6"/>
     </row>
-    <row r="504" spans="2:2" ht="12">
+    <row r="504" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B504" s="6"/>
     </row>
-    <row r="505" spans="2:2" ht="12">
+    <row r="505" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B505" s="6"/>
     </row>
-    <row r="506" spans="2:2" ht="12">
+    <row r="506" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B506" s="6"/>
     </row>
-    <row r="507" spans="2:2" ht="12">
+    <row r="507" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B507" s="6"/>
     </row>
-    <row r="508" spans="2:2" ht="12">
+    <row r="508" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B508" s="6"/>
     </row>
-    <row r="509" spans="2:2" ht="12">
+    <row r="509" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B509" s="6"/>
     </row>
-    <row r="510" spans="2:2" ht="12">
+    <row r="510" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B510" s="6"/>
     </row>
-    <row r="511" spans="2:2" ht="12">
+    <row r="511" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B511" s="6"/>
     </row>
-    <row r="512" spans="2:2" ht="12">
+    <row r="512" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B512" s="6"/>
     </row>
-    <row r="513" spans="2:2" ht="12">
+    <row r="513" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B513" s="6"/>
     </row>
-    <row r="514" spans="2:2" ht="12">
+    <row r="514" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B514" s="6"/>
     </row>
-    <row r="515" spans="2:2" ht="12">
+    <row r="515" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B515" s="6"/>
     </row>
-    <row r="516" spans="2:2" ht="12">
+    <row r="516" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B516" s="6"/>
     </row>
-    <row r="517" spans="2:2" ht="12">
+    <row r="517" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B517" s="6"/>
     </row>
-    <row r="518" spans="2:2" ht="12">
+    <row r="518" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B518" s="6"/>
     </row>
-    <row r="519" spans="2:2" ht="12">
+    <row r="519" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B519" s="6"/>
     </row>
-    <row r="520" spans="2:2" ht="12">
+    <row r="520" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B520" s="6"/>
     </row>
-    <row r="521" spans="2:2" ht="12">
+    <row r="521" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B521" s="6"/>
     </row>
-    <row r="522" spans="2:2" ht="12">
+    <row r="522" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B522" s="6"/>
     </row>
-    <row r="523" spans="2:2" ht="12">
+    <row r="523" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B523" s="6"/>
     </row>
-    <row r="524" spans="2:2" ht="12">
+    <row r="524" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B524" s="6"/>
     </row>
-    <row r="525" spans="2:2" ht="12">
+    <row r="525" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B525" s="6"/>
     </row>
-    <row r="526" spans="2:2" ht="12">
+    <row r="526" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B526" s="6"/>
     </row>
-    <row r="527" spans="2:2" ht="12">
+    <row r="527" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B527" s="6"/>
     </row>
-    <row r="528" spans="2:2" ht="12">
+    <row r="528" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B528" s="6"/>
     </row>
-    <row r="529" spans="2:2" ht="12">
+    <row r="529" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B529" s="6"/>
     </row>
-    <row r="530" spans="2:2" ht="12">
+    <row r="530" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B530" s="6"/>
     </row>
-    <row r="531" spans="2:2" ht="12">
+    <row r="531" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B531" s="6"/>
     </row>
-    <row r="532" spans="2:2" ht="12">
+    <row r="532" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B532" s="6"/>
     </row>
-    <row r="533" spans="2:2" ht="12">
+    <row r="533" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B533" s="6"/>
     </row>
-    <row r="534" spans="2:2" ht="12">
+    <row r="534" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B534" s="6"/>
     </row>
-    <row r="535" spans="2:2" ht="12">
+    <row r="535" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B535" s="6"/>
     </row>
-    <row r="536" spans="2:2" ht="12">
+    <row r="536" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B536" s="6"/>
     </row>
-    <row r="537" spans="2:2" ht="12">
+    <row r="537" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B537" s="6"/>
     </row>
-    <row r="538" spans="2:2" ht="12">
+    <row r="538" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B538" s="6"/>
     </row>
-    <row r="539" spans="2:2" ht="12">
+    <row r="539" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B539" s="6"/>
     </row>
-    <row r="540" spans="2:2" ht="12">
+    <row r="540" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B540" s="6"/>
     </row>
-    <row r="541" spans="2:2" ht="12">
+    <row r="541" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B541" s="6"/>
     </row>
-    <row r="542" spans="2:2" ht="12">
+    <row r="542" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B542" s="6"/>
     </row>
-    <row r="543" spans="2:2" ht="12">
+    <row r="543" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B543" s="6"/>
     </row>
-    <row r="544" spans="2:2" ht="12">
+    <row r="544" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B544" s="6"/>
     </row>
-    <row r="545" spans="2:2" ht="12">
+    <row r="545" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B545" s="6"/>
     </row>
-    <row r="546" spans="2:2" ht="12">
+    <row r="546" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B546" s="6"/>
     </row>
-    <row r="547" spans="2:2" ht="12">
+    <row r="547" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B547" s="6"/>
     </row>
-    <row r="548" spans="2:2" ht="12">
+    <row r="548" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B548" s="6"/>
     </row>
-    <row r="549" spans="2:2" ht="12">
+    <row r="549" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B549" s="6"/>
     </row>
-    <row r="550" spans="2:2" ht="12">
+    <row r="550" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B550" s="6"/>
     </row>
-    <row r="551" spans="2:2" ht="12">
+    <row r="551" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B551" s="6"/>
     </row>
-    <row r="552" spans="2:2" ht="12">
+    <row r="552" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B552" s="6"/>
     </row>
-    <row r="553" spans="2:2" ht="12">
+    <row r="553" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B553" s="6"/>
     </row>
-    <row r="554" spans="2:2" ht="12">
+    <row r="554" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B554" s="6"/>
     </row>
-    <row r="555" spans="2:2" ht="12">
+    <row r="555" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B555" s="6"/>
     </row>
-    <row r="556" spans="2:2" ht="12">
+    <row r="556" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B556" s="6"/>
     </row>
-    <row r="557" spans="2:2" ht="12">
+    <row r="557" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B557" s="6"/>
     </row>
-    <row r="558" spans="2:2" ht="12">
+    <row r="558" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B558" s="6"/>
     </row>
-    <row r="559" spans="2:2" ht="12">
+    <row r="559" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B559" s="6"/>
     </row>
-    <row r="560" spans="2:2" ht="12">
+    <row r="560" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B560" s="6"/>
     </row>
-    <row r="561" spans="2:2" ht="12">
+    <row r="561" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B561" s="6"/>
     </row>
-    <row r="562" spans="2:2" ht="12">
+    <row r="562" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B562" s="6"/>
     </row>
-    <row r="563" spans="2:2" ht="12">
+    <row r="563" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B563" s="6"/>
     </row>
-    <row r="564" spans="2:2" ht="12">
+    <row r="564" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B564" s="6"/>
     </row>
-    <row r="565" spans="2:2" ht="12">
+    <row r="565" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B565" s="6"/>
     </row>
-    <row r="566" spans="2:2" ht="12">
+    <row r="566" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B566" s="6"/>
     </row>
-    <row r="567" spans="2:2" ht="12">
+    <row r="567" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B567" s="6"/>
     </row>
-    <row r="568" spans="2:2" ht="12">
+    <row r="568" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B568" s="6"/>
     </row>
-    <row r="569" spans="2:2" ht="12">
+    <row r="569" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B569" s="6"/>
     </row>
-    <row r="570" spans="2:2" ht="12">
+    <row r="570" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B570" s="6"/>
     </row>
-    <row r="571" spans="2:2" ht="12">
+    <row r="571" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B571" s="6"/>
     </row>
-    <row r="572" spans="2:2" ht="12">
+    <row r="572" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B572" s="6"/>
     </row>
-    <row r="573" spans="2:2" ht="12">
+    <row r="573" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B573" s="6"/>
     </row>
-    <row r="574" spans="2:2" ht="12">
+    <row r="574" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B574" s="6"/>
     </row>
-    <row r="575" spans="2:2" ht="12">
+    <row r="575" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B575" s="6"/>
     </row>
-    <row r="576" spans="2:2" ht="12">
+    <row r="576" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B576" s="6"/>
     </row>
-    <row r="577" spans="2:2" ht="12">
+    <row r="577" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B577" s="6"/>
     </row>
-    <row r="578" spans="2:2" ht="12">
+    <row r="578" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B578" s="6"/>
     </row>
-    <row r="579" spans="2:2" ht="12">
+    <row r="579" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B579" s="6"/>
     </row>
-    <row r="580" spans="2:2" ht="12">
+    <row r="580" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B580" s="6"/>
     </row>
-    <row r="581" spans="2:2" ht="12">
+    <row r="581" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B581" s="6"/>
     </row>
-    <row r="582" spans="2:2" ht="12">
+    <row r="582" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B582" s="6"/>
     </row>
-    <row r="583" spans="2:2" ht="12">
+    <row r="583" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B583" s="6"/>
     </row>
-    <row r="584" spans="2:2" ht="12">
+    <row r="584" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B584" s="6"/>
     </row>
-    <row r="585" spans="2:2" ht="12">
+    <row r="585" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B585" s="6"/>
     </row>
-    <row r="586" spans="2:2" ht="12">
+    <row r="586" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B586" s="6"/>
     </row>
-    <row r="587" spans="2:2" ht="12">
+    <row r="587" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B587" s="6"/>
     </row>
-    <row r="588" spans="2:2" ht="12">
+    <row r="588" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B588" s="6"/>
     </row>
-    <row r="589" spans="2:2" ht="12">
+    <row r="589" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B589" s="6"/>
     </row>
-    <row r="590" spans="2:2" ht="12">
+    <row r="590" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B590" s="6"/>
     </row>
-    <row r="591" spans="2:2" ht="12">
+    <row r="591" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B591" s="6"/>
     </row>
-    <row r="592" spans="2:2" ht="12">
+    <row r="592" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B592" s="6"/>
     </row>
-    <row r="593" spans="2:2" ht="12">
+    <row r="593" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B593" s="6"/>
     </row>
-    <row r="594" spans="2:2" ht="12">
+    <row r="594" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B594" s="6"/>
     </row>
-    <row r="595" spans="2:2" ht="12">
+    <row r="595" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B595" s="6"/>
     </row>
-    <row r="596" spans="2:2" ht="12">
+    <row r="596" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B596" s="6"/>
     </row>
-    <row r="597" spans="2:2" ht="12">
+    <row r="597" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B597" s="6"/>
     </row>
-    <row r="598" spans="2:2" ht="12">
+    <row r="598" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B598" s="6"/>
     </row>
-    <row r="599" spans="2:2" ht="12">
+    <row r="599" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B599" s="6"/>
     </row>
-    <row r="600" spans="2:2" ht="12">
+    <row r="600" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B600" s="6"/>
     </row>
-    <row r="601" spans="2:2" ht="12">
+    <row r="601" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B601" s="6"/>
     </row>
-    <row r="602" spans="2:2" ht="12">
+    <row r="602" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B602" s="6"/>
     </row>
-    <row r="603" spans="2:2" ht="12">
+    <row r="603" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B603" s="6"/>
     </row>
-    <row r="604" spans="2:2" ht="12">
+    <row r="604" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B604" s="6"/>
     </row>
-    <row r="605" spans="2:2" ht="12">
+    <row r="605" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B605" s="6"/>
     </row>
-    <row r="606" spans="2:2" ht="12">
+    <row r="606" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B606" s="6"/>
     </row>
-    <row r="607" spans="2:2" ht="12">
+    <row r="607" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B607" s="6"/>
     </row>
-    <row r="608" spans="2:2" ht="12">
+    <row r="608" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B608" s="6"/>
     </row>
-    <row r="609" spans="2:2" ht="12">
+    <row r="609" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B609" s="6"/>
     </row>
-    <row r="610" spans="2:2" ht="12">
+    <row r="610" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B610" s="6"/>
     </row>
-    <row r="611" spans="2:2" ht="12">
+    <row r="611" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B611" s="6"/>
     </row>
-    <row r="612" spans="2:2" ht="12">
+    <row r="612" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B612" s="6"/>
     </row>
-    <row r="613" spans="2:2" ht="12">
+    <row r="613" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B613" s="6"/>
     </row>
-    <row r="614" spans="2:2" ht="12">
+    <row r="614" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B614" s="6"/>
     </row>
-    <row r="615" spans="2:2" ht="12">
+    <row r="615" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B615" s="6"/>
     </row>
-    <row r="616" spans="2:2" ht="12">
+    <row r="616" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B616" s="6"/>
     </row>
-    <row r="617" spans="2:2" ht="12">
+    <row r="617" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B617" s="6"/>
     </row>
-    <row r="618" spans="2:2" ht="12">
+    <row r="618" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B618" s="6"/>
     </row>
-    <row r="619" spans="2:2" ht="12">
+    <row r="619" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B619" s="6"/>
     </row>
-    <row r="620" spans="2:2" ht="12">
+    <row r="620" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B620" s="6"/>
     </row>
-    <row r="621" spans="2:2" ht="12">
+    <row r="621" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B621" s="6"/>
     </row>
-    <row r="622" spans="2:2" ht="12">
+    <row r="622" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B622" s="6"/>
     </row>
-    <row r="623" spans="2:2" ht="12">
+    <row r="623" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B623" s="6"/>
     </row>
-    <row r="624" spans="2:2" ht="12">
+    <row r="624" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B624" s="6"/>
     </row>
-    <row r="625" spans="2:2" ht="12">
+    <row r="625" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B625" s="6"/>
     </row>
-    <row r="626" spans="2:2" ht="12">
+    <row r="626" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B626" s="6"/>
     </row>
-    <row r="627" spans="2:2" ht="12">
+    <row r="627" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B627" s="6"/>
     </row>
-    <row r="628" spans="2:2" ht="12">
+    <row r="628" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B628" s="6"/>
     </row>
-    <row r="629" spans="2:2" ht="12">
+    <row r="629" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B629" s="6"/>
     </row>
-    <row r="630" spans="2:2" ht="12">
+    <row r="630" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B630" s="6"/>
     </row>
-    <row r="631" spans="2:2" ht="12">
+    <row r="631" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B631" s="6"/>
     </row>
-    <row r="632" spans="2:2" ht="12">
+    <row r="632" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B632" s="6"/>
     </row>
-    <row r="633" spans="2:2" ht="12">
+    <row r="633" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B633" s="6"/>
     </row>
-    <row r="634" spans="2:2" ht="12">
+    <row r="634" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B634" s="6"/>
     </row>
-    <row r="635" spans="2:2" ht="12">
+    <row r="635" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B635" s="6"/>
     </row>
-    <row r="636" spans="2:2" ht="12">
+    <row r="636" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B636" s="6"/>
     </row>
-    <row r="637" spans="2:2" ht="12">
+    <row r="637" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B637" s="6"/>
     </row>
-    <row r="638" spans="2:2" ht="12">
+    <row r="638" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B638" s="6"/>
     </row>
-    <row r="639" spans="2:2" ht="12">
+    <row r="639" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B639" s="6"/>
     </row>
-    <row r="640" spans="2:2" ht="12">
+    <row r="640" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B640" s="6"/>
     </row>
-    <row r="641" spans="2:2" ht="12">
+    <row r="641" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B641" s="6"/>
     </row>
-    <row r="642" spans="2:2" ht="12">
+    <row r="642" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B642" s="6"/>
     </row>
-    <row r="643" spans="2:2" ht="12">
+    <row r="643" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B643" s="6"/>
     </row>
-    <row r="644" spans="2:2" ht="12">
+    <row r="644" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B644" s="6"/>
     </row>
-    <row r="645" spans="2:2" ht="12">
+    <row r="645" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B645" s="6"/>
     </row>
-    <row r="646" spans="2:2" ht="12">
+    <row r="646" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B646" s="6"/>
     </row>
-    <row r="647" spans="2:2" ht="12">
+    <row r="647" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B647" s="6"/>
     </row>
-    <row r="648" spans="2:2" ht="12">
+    <row r="648" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B648" s="6"/>
     </row>
-    <row r="649" spans="2:2" ht="12">
+    <row r="649" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B649" s="6"/>
     </row>
-    <row r="650" spans="2:2" ht="12">
+    <row r="650" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B650" s="6"/>
     </row>
-    <row r="651" spans="2:2" ht="12">
+    <row r="651" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B651" s="6"/>
     </row>
-    <row r="652" spans="2:2" ht="12">
+    <row r="652" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B652" s="6"/>
     </row>
-    <row r="653" spans="2:2" ht="12">
+    <row r="653" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B653" s="6"/>
     </row>
-    <row r="654" spans="2:2" ht="12">
+    <row r="654" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B654" s="6"/>
     </row>
-    <row r="655" spans="2:2" ht="12">
+    <row r="655" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B655" s="6"/>
     </row>
-    <row r="656" spans="2:2" ht="12">
+    <row r="656" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B656" s="6"/>
     </row>
-    <row r="657" spans="2:2" ht="12">
+    <row r="657" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B657" s="6"/>
     </row>
-    <row r="658" spans="2:2" ht="12">
+    <row r="658" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B658" s="6"/>
     </row>
-    <row r="659" spans="2:2" ht="12">
+    <row r="659" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B659" s="6"/>
     </row>
-    <row r="660" spans="2:2" ht="12">
+    <row r="660" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B660" s="6"/>
     </row>
-    <row r="661" spans="2:2" ht="12">
+    <row r="661" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B661" s="6"/>
     </row>
-    <row r="662" spans="2:2" ht="12">
+    <row r="662" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B662" s="6"/>
     </row>
-    <row r="663" spans="2:2" ht="12">
+    <row r="663" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B663" s="6"/>
     </row>
-    <row r="664" spans="2:2" ht="12">
+    <row r="664" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B664" s="6"/>
     </row>
-    <row r="665" spans="2:2" ht="12">
+    <row r="665" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B665" s="6"/>
     </row>
-    <row r="666" spans="2:2" ht="12">
+    <row r="666" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B666" s="6"/>
     </row>
-    <row r="667" spans="2:2" ht="12">
+    <row r="667" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B667" s="6"/>
     </row>
-    <row r="668" spans="2:2" ht="12">
+    <row r="668" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B668" s="6"/>
     </row>
-    <row r="669" spans="2:2" ht="12">
+    <row r="669" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B669" s="6"/>
     </row>
-    <row r="670" spans="2:2" ht="12">
+    <row r="670" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B670" s="6"/>
     </row>
-    <row r="671" spans="2:2" ht="12">
+    <row r="671" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B671" s="6"/>
     </row>
-    <row r="672" spans="2:2" ht="12">
+    <row r="672" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B672" s="6"/>
     </row>
-    <row r="673" spans="2:2" ht="12">
+    <row r="673" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B673" s="6"/>
     </row>
-    <row r="674" spans="2:2" ht="12">
+    <row r="674" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B674" s="6"/>
     </row>
-    <row r="675" spans="2:2" ht="12">
+    <row r="675" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B675" s="6"/>
     </row>
-    <row r="676" spans="2:2" ht="12">
+    <row r="676" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B676" s="6"/>
     </row>
-    <row r="677" spans="2:2" ht="12">
+    <row r="677" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B677" s="6"/>
     </row>
-    <row r="678" spans="2:2" ht="12">
+    <row r="678" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B678" s="6"/>
     </row>
-    <row r="679" spans="2:2" ht="12">
+    <row r="679" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B679" s="6"/>
     </row>
-    <row r="680" spans="2:2" ht="12">
+    <row r="680" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B680" s="6"/>
     </row>
-    <row r="681" spans="2:2" ht="12">
+    <row r="681" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B681" s="6"/>
     </row>
-    <row r="682" spans="2:2" ht="12">
+    <row r="682" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B682" s="6"/>
     </row>
-    <row r="683" spans="2:2" ht="12">
+    <row r="683" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B683" s="6"/>
     </row>
-    <row r="684" spans="2:2" ht="12">
+    <row r="684" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B684" s="6"/>
     </row>
-    <row r="685" spans="2:2" ht="12">
+    <row r="685" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B685" s="6"/>
     </row>
-    <row r="686" spans="2:2" ht="12">
+    <row r="686" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B686" s="6"/>
     </row>
-    <row r="687" spans="2:2" ht="12">
+    <row r="687" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B687" s="6"/>
     </row>
-    <row r="688" spans="2:2" ht="12">
+    <row r="688" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B688" s="6"/>
     </row>
-    <row r="689" spans="2:2" ht="12">
+    <row r="689" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B689" s="6"/>
     </row>
-    <row r="690" spans="2:2" ht="12">
+    <row r="690" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B690" s="6"/>
     </row>
-    <row r="691" spans="2:2" ht="12">
+    <row r="691" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B691" s="6"/>
     </row>
-    <row r="692" spans="2:2" ht="12">
+    <row r="692" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B692" s="6"/>
     </row>
-    <row r="693" spans="2:2" ht="12">
+    <row r="693" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B693" s="6"/>
     </row>
-    <row r="694" spans="2:2" ht="12">
+    <row r="694" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B694" s="6"/>
     </row>
-    <row r="695" spans="2:2" ht="12">
+    <row r="695" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B695" s="6"/>
     </row>
-    <row r="696" spans="2:2" ht="12">
+    <row r="696" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B696" s="6"/>
     </row>
-    <row r="697" spans="2:2" ht="12">
+    <row r="697" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B697" s="6"/>
     </row>
-    <row r="698" spans="2:2" ht="12">
+    <row r="698" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B698" s="6"/>
     </row>
-    <row r="699" spans="2:2" ht="12">
+    <row r="699" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B699" s="6"/>
     </row>
-    <row r="700" spans="2:2" ht="12">
+    <row r="700" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B700" s="6"/>
     </row>
-    <row r="701" spans="2:2" ht="12">
+    <row r="701" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B701" s="6"/>
     </row>
-    <row r="702" spans="2:2" ht="12">
+    <row r="702" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B702" s="6"/>
     </row>
-    <row r="703" spans="2:2" ht="12">
+    <row r="703" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B703" s="6"/>
     </row>
-    <row r="704" spans="2:2" ht="12">
+    <row r="704" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B704" s="6"/>
     </row>
-    <row r="705" spans="2:2" ht="12">
+    <row r="705" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B705" s="6"/>
     </row>
-    <row r="706" spans="2:2" ht="12">
+    <row r="706" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B706" s="6"/>
     </row>
-    <row r="707" spans="2:2" ht="12">
+    <row r="707" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B707" s="6"/>
     </row>
-    <row r="708" spans="2:2" ht="12">
+    <row r="708" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B708" s="6"/>
     </row>
-    <row r="709" spans="2:2" ht="12">
+    <row r="709" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B709" s="6"/>
     </row>
-    <row r="710" spans="2:2" ht="12">
+    <row r="710" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B710" s="6"/>
     </row>
-    <row r="711" spans="2:2" ht="12">
+    <row r="711" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B711" s="6"/>
     </row>
-    <row r="712" spans="2:2" ht="12">
+    <row r="712" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B712" s="6"/>
     </row>
-    <row r="713" spans="2:2" ht="12">
+    <row r="713" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B713" s="6"/>
     </row>
-    <row r="714" spans="2:2" ht="12">
+    <row r="714" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B714" s="6"/>
     </row>
-    <row r="715" spans="2:2" ht="12">
+    <row r="715" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B715" s="6"/>
     </row>
-    <row r="716" spans="2:2" ht="12">
+    <row r="716" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B716" s="6"/>
     </row>
-    <row r="717" spans="2:2" ht="12">
+    <row r="717" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B717" s="6"/>
     </row>
-    <row r="718" spans="2:2" ht="12">
+    <row r="718" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B718" s="6"/>
     </row>
-    <row r="719" spans="2:2" ht="12">
+    <row r="719" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B719" s="6"/>
     </row>
-    <row r="720" spans="2:2" ht="12">
+    <row r="720" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B720" s="6"/>
     </row>
-    <row r="721" spans="2:2" ht="12">
+    <row r="721" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B721" s="6"/>
     </row>
-    <row r="722" spans="2:2" ht="12">
+    <row r="722" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B722" s="6"/>
     </row>
-    <row r="723" spans="2:2" ht="12">
+    <row r="723" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B723" s="6"/>
     </row>
-    <row r="724" spans="2:2" ht="12">
+    <row r="724" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B724" s="6"/>
     </row>
-    <row r="725" spans="2:2" ht="12">
+    <row r="725" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B725" s="6"/>
     </row>
-    <row r="726" spans="2:2" ht="12">
+    <row r="726" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B726" s="6"/>
     </row>
-    <row r="727" spans="2:2" ht="12">
+    <row r="727" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B727" s="6"/>
     </row>
-    <row r="728" spans="2:2" ht="12">
+    <row r="728" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B728" s="6"/>
     </row>
-    <row r="729" spans="2:2" ht="12">
+    <row r="729" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B729" s="6"/>
     </row>
-    <row r="730" spans="2:2" ht="12">
+    <row r="730" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B730" s="6"/>
     </row>
-    <row r="731" spans="2:2" ht="12">
+    <row r="731" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B731" s="6"/>
     </row>
-    <row r="732" spans="2:2" ht="12">
+    <row r="732" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B732" s="6"/>
     </row>
-    <row r="733" spans="2:2" ht="12">
+    <row r="733" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B733" s="6"/>
     </row>
-    <row r="734" spans="2:2" ht="12">
+    <row r="734" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B734" s="6"/>
     </row>
-    <row r="735" spans="2:2" ht="12">
+    <row r="735" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B735" s="6"/>
     </row>
-    <row r="736" spans="2:2" ht="12">
+    <row r="736" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B736" s="6"/>
     </row>
-    <row r="737" spans="2:2" ht="12">
+    <row r="737" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B737" s="6"/>
     </row>
-    <row r="738" spans="2:2" ht="12">
+    <row r="738" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B738" s="6"/>
     </row>
-    <row r="739" spans="2:2" ht="12">
+    <row r="739" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B739" s="6"/>
     </row>
-    <row r="740" spans="2:2" ht="12">
+    <row r="740" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B740" s="6"/>
     </row>
-    <row r="741" spans="2:2" ht="12">
+    <row r="741" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B741" s="6"/>
     </row>
-    <row r="742" spans="2:2" ht="12">
+    <row r="742" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B742" s="6"/>
     </row>
-    <row r="743" spans="2:2" ht="12">
+    <row r="743" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B743" s="6"/>
     </row>
-    <row r="744" spans="2:2" ht="12">
+    <row r="744" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B744" s="6"/>
     </row>
-    <row r="745" spans="2:2" ht="12">
+    <row r="745" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B745" s="6"/>
     </row>
-    <row r="746" spans="2:2" ht="12">
+    <row r="746" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B746" s="6"/>
     </row>
-    <row r="747" spans="2:2" ht="12">
+    <row r="747" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B747" s="6"/>
     </row>
-    <row r="748" spans="2:2" ht="12">
+    <row r="748" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B748" s="6"/>
     </row>
-    <row r="749" spans="2:2" ht="12">
+    <row r="749" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B749" s="6"/>
     </row>
-    <row r="750" spans="2:2" ht="12">
+    <row r="750" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B750" s="6"/>
     </row>
-    <row r="751" spans="2:2" ht="12">
+    <row r="751" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B751" s="6"/>
     </row>
-    <row r="752" spans="2:2" ht="12">
+    <row r="752" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B752" s="6"/>
     </row>
-    <row r="753" spans="2:2" ht="12">
+    <row r="753" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B753" s="6"/>
     </row>
-    <row r="754" spans="2:2" ht="12">
+    <row r="754" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B754" s="6"/>
     </row>
-    <row r="755" spans="2:2" ht="12">
+    <row r="755" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B755" s="6"/>
     </row>
-    <row r="756" spans="2:2" ht="12">
+    <row r="756" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B756" s="6"/>
     </row>
-    <row r="757" spans="2:2" ht="12">
+    <row r="757" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B757" s="6"/>
     </row>
-    <row r="758" spans="2:2" ht="12">
+    <row r="758" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B758" s="6"/>
     </row>
-    <row r="759" spans="2:2" ht="12">
+    <row r="759" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B759" s="6"/>
     </row>
-    <row r="760" spans="2:2" ht="12">
+    <row r="760" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B760" s="6"/>
     </row>
-    <row r="761" spans="2:2" ht="12">
+    <row r="761" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B761" s="6"/>
     </row>
-    <row r="762" spans="2:2" ht="12">
+    <row r="762" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B762" s="6"/>
     </row>
-    <row r="763" spans="2:2" ht="12">
+    <row r="763" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B763" s="6"/>
     </row>
-    <row r="764" spans="2:2" ht="12">
+    <row r="764" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B764" s="6"/>
     </row>
-    <row r="765" spans="2:2" ht="12">
+    <row r="765" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B765" s="6"/>
     </row>
-    <row r="766" spans="2:2" ht="12">
+    <row r="766" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B766" s="6"/>
     </row>
-    <row r="767" spans="2:2" ht="12">
+    <row r="767" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B767" s="6"/>
     </row>
-    <row r="768" spans="2:2" ht="12">
+    <row r="768" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B768" s="6"/>
     </row>
-    <row r="769" spans="2:2" ht="12">
+    <row r="769" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B769" s="6"/>
     </row>
-    <row r="770" spans="2:2" ht="12">
+    <row r="770" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B770" s="6"/>
     </row>
-    <row r="771" spans="2:2" ht="12">
+    <row r="771" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B771" s="6"/>
     </row>
-    <row r="772" spans="2:2" ht="12">
+    <row r="772" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B772" s="6"/>
     </row>
-    <row r="773" spans="2:2" ht="12">
+    <row r="773" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B773" s="6"/>
     </row>
-    <row r="774" spans="2:2" ht="12">
+    <row r="774" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B774" s="6"/>
     </row>
-    <row r="775" spans="2:2" ht="12">
+    <row r="775" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B775" s="6"/>
     </row>
-    <row r="776" spans="2:2" ht="12">
+    <row r="776" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B776" s="6"/>
     </row>
-    <row r="777" spans="2:2" ht="12">
+    <row r="777" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B777" s="6"/>
     </row>
-    <row r="778" spans="2:2" ht="12">
+    <row r="778" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B778" s="6"/>
     </row>
-    <row r="779" spans="2:2" ht="12">
+    <row r="779" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B779" s="6"/>
     </row>
-    <row r="780" spans="2:2" ht="12">
+    <row r="780" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B780" s="6"/>
     </row>
-    <row r="781" spans="2:2" ht="12">
+    <row r="781" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B781" s="6"/>
     </row>
-    <row r="782" spans="2:2" ht="12">
+    <row r="782" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B782" s="6"/>
     </row>
-    <row r="783" spans="2:2" ht="12">
+    <row r="783" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B783" s="6"/>
     </row>
-    <row r="784" spans="2:2" ht="12">
+    <row r="784" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B784" s="6"/>
     </row>
-    <row r="785" spans="2:2" ht="12">
+    <row r="785" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B785" s="6"/>
     </row>
-    <row r="786" spans="2:2" ht="12">
+    <row r="786" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B786" s="6"/>
     </row>
-    <row r="787" spans="2:2" ht="12">
+    <row r="787" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B787" s="6"/>
     </row>
-    <row r="788" spans="2:2" ht="12">
+    <row r="788" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B788" s="6"/>
     </row>
-    <row r="789" spans="2:2" ht="12">
+    <row r="789" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B789" s="6"/>
     </row>
-    <row r="790" spans="2:2" ht="12">
+    <row r="790" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B790" s="6"/>
     </row>
-    <row r="791" spans="2:2" ht="12">
+    <row r="791" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B791" s="6"/>
     </row>
-    <row r="792" spans="2:2" ht="12">
+    <row r="792" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B792" s="6"/>
     </row>
-    <row r="793" spans="2:2" ht="12">
+    <row r="793" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B793" s="6"/>
     </row>
-    <row r="794" spans="2:2" ht="12">
+    <row r="794" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B794" s="6"/>
     </row>
-    <row r="795" spans="2:2" ht="12">
+    <row r="795" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B795" s="6"/>
     </row>
-    <row r="796" spans="2:2" ht="12">
+    <row r="796" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B796" s="6"/>
     </row>
-    <row r="797" spans="2:2" ht="12">
+    <row r="797" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B797" s="6"/>
     </row>
-    <row r="798" spans="2:2" ht="12">
+    <row r="798" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B798" s="6"/>
     </row>
-    <row r="799" spans="2:2" ht="12">
+    <row r="799" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B799" s="6"/>
     </row>
-    <row r="800" spans="2:2" ht="12">
+    <row r="800" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B800" s="6"/>
     </row>
-    <row r="801" spans="2:2" ht="12">
+    <row r="801" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B801" s="6"/>
     </row>
-    <row r="802" spans="2:2" ht="12">
+    <row r="802" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B802" s="6"/>
     </row>
-    <row r="803" spans="2:2" ht="12">
+    <row r="803" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B803" s="6"/>
     </row>
-    <row r="804" spans="2:2" ht="12">
+    <row r="804" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B804" s="6"/>
     </row>
-    <row r="805" spans="2:2" ht="12">
+    <row r="805" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B805" s="6"/>
     </row>
-    <row r="806" spans="2:2" ht="12">
+    <row r="806" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B806" s="6"/>
     </row>
-    <row r="807" spans="2:2" ht="12">
+    <row r="807" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B807" s="6"/>
     </row>
-    <row r="808" spans="2:2" ht="12">
+    <row r="808" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B808" s="6"/>
     </row>
-    <row r="809" spans="2:2" ht="12">
+    <row r="809" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B809" s="6"/>
     </row>
-    <row r="810" spans="2:2" ht="12">
+    <row r="810" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B810" s="6"/>
     </row>
-    <row r="811" spans="2:2" ht="12">
+    <row r="811" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B811" s="6"/>
     </row>
-    <row r="812" spans="2:2" ht="12">
+    <row r="812" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B812" s="6"/>
     </row>
-    <row r="813" spans="2:2" ht="12">
+    <row r="813" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B813" s="6"/>
     </row>
-    <row r="814" spans="2:2" ht="12">
+    <row r="814" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B814" s="6"/>
     </row>
-    <row r="815" spans="2:2" ht="12">
+    <row r="815" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B815" s="6"/>
     </row>
-    <row r="816" spans="2:2" ht="12">
+    <row r="816" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B816" s="6"/>
     </row>
-    <row r="817" spans="2:2" ht="12">
+    <row r="817" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B817" s="6"/>
     </row>
-    <row r="818" spans="2:2" ht="12">
+    <row r="818" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B818" s="6"/>
     </row>
-    <row r="819" spans="2:2" ht="12">
+    <row r="819" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B819" s="6"/>
     </row>
-    <row r="820" spans="2:2" ht="12">
+    <row r="820" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B820" s="6"/>
     </row>
-    <row r="821" spans="2:2" ht="12">
+    <row r="821" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B821" s="6"/>
     </row>
-    <row r="822" spans="2:2" ht="12">
+    <row r="822" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B822" s="6"/>
     </row>
-    <row r="823" spans="2:2" ht="12">
+    <row r="823" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B823" s="6"/>
     </row>
-    <row r="824" spans="2:2" ht="12">
+    <row r="824" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B824" s="6"/>
     </row>
-    <row r="825" spans="2:2" ht="12">
+    <row r="825" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B825" s="6"/>
     </row>
-    <row r="826" spans="2:2" ht="12">
+    <row r="826" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B826" s="6"/>
     </row>
-    <row r="827" spans="2:2" ht="12">
+    <row r="827" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B827" s="6"/>
     </row>
-    <row r="828" spans="2:2" ht="12">
+    <row r="828" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B828" s="6"/>
     </row>
-    <row r="829" spans="2:2" ht="12">
+    <row r="829" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B829" s="6"/>
     </row>
-    <row r="830" spans="2:2" ht="12">
+    <row r="830" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B830" s="6"/>
     </row>
-    <row r="831" spans="2:2" ht="12">
+    <row r="831" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B831" s="6"/>
     </row>
-    <row r="832" spans="2:2" ht="12">
+    <row r="832" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B832" s="6"/>
     </row>
-    <row r="833" spans="2:2" ht="12">
+    <row r="833" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B833" s="6"/>
     </row>
-    <row r="834" spans="2:2" ht="12">
+    <row r="834" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B834" s="6"/>
     </row>
-    <row r="835" spans="2:2" ht="12">
+    <row r="835" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B835" s="6"/>
     </row>
-    <row r="836" spans="2:2" ht="12">
+    <row r="836" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B836" s="6"/>
     </row>
-    <row r="837" spans="2:2" ht="12">
+    <row r="837" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B837" s="6"/>
     </row>
-    <row r="838" spans="2:2" ht="12">
+    <row r="838" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B838" s="6"/>
     </row>
-    <row r="839" spans="2:2" ht="12">
+    <row r="839" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B839" s="6"/>
     </row>
-    <row r="840" spans="2:2" ht="12">
+    <row r="840" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B840" s="6"/>
     </row>
-    <row r="841" spans="2:2" ht="12">
+    <row r="841" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B841" s="6"/>
     </row>
-    <row r="842" spans="2:2" ht="12">
+    <row r="842" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B842" s="6"/>
     </row>
-    <row r="843" spans="2:2" ht="12">
+    <row r="843" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B843" s="6"/>
     </row>
-    <row r="844" spans="2:2" ht="12">
+    <row r="844" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B844" s="6"/>
     </row>
-    <row r="845" spans="2:2" ht="12">
+    <row r="845" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B845" s="6"/>
     </row>
-    <row r="846" spans="2:2" ht="12">
+    <row r="846" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B846" s="6"/>
     </row>
-    <row r="847" spans="2:2" ht="12">
+    <row r="847" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B847" s="6"/>
     </row>
-    <row r="848" spans="2:2" ht="12">
+    <row r="848" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B848" s="6"/>
     </row>
-    <row r="849" spans="2:2" ht="12">
+    <row r="849" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B849" s="6"/>
     </row>
-    <row r="850" spans="2:2" ht="12">
+    <row r="850" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B850" s="6"/>
     </row>
-    <row r="851" spans="2:2" ht="12">
+    <row r="851" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B851" s="6"/>
     </row>
-    <row r="852" spans="2:2" ht="12">
+    <row r="852" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B852" s="6"/>
     </row>
-    <row r="853" spans="2:2" ht="12">
+    <row r="853" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B853" s="6"/>
     </row>
-    <row r="854" spans="2:2" ht="12">
+    <row r="854" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B854" s="6"/>
     </row>
-    <row r="855" spans="2:2" ht="12">
+    <row r="855" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B855" s="6"/>
     </row>
-    <row r="856" spans="2:2" ht="12">
+    <row r="856" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B856" s="6"/>
     </row>
-    <row r="857" spans="2:2" ht="12">
+    <row r="857" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B857" s="6"/>
     </row>
-    <row r="858" spans="2:2" ht="12">
+    <row r="858" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B858" s="6"/>
     </row>
-    <row r="859" spans="2:2" ht="12">
+    <row r="859" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B859" s="6"/>
     </row>
-    <row r="860" spans="2:2" ht="12">
+    <row r="860" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B860" s="6"/>
     </row>
-    <row r="861" spans="2:2" ht="12">
+    <row r="861" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B861" s="6"/>
     </row>
-    <row r="862" spans="2:2" ht="12">
+    <row r="862" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B862" s="6"/>
     </row>
-    <row r="863" spans="2:2" ht="12">
+    <row r="863" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B863" s="6"/>
     </row>
-    <row r="864" spans="2:2" ht="12">
+    <row r="864" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B864" s="6"/>
     </row>
-    <row r="865" spans="2:2" ht="12">
+    <row r="865" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B865" s="6"/>
     </row>
-    <row r="866" spans="2:2" ht="12">
+    <row r="866" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B866" s="6"/>
     </row>
-    <row r="867" spans="2:2" ht="12">
+    <row r="867" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B867" s="6"/>
     </row>
-    <row r="868" spans="2:2" ht="12">
+    <row r="868" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B868" s="6"/>
     </row>
-    <row r="869" spans="2:2" ht="12">
+    <row r="869" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B869" s="6"/>
     </row>
-    <row r="870" spans="2:2" ht="12">
+    <row r="870" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B870" s="6"/>
     </row>
-    <row r="871" spans="2:2" ht="12">
+    <row r="871" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B871" s="6"/>
     </row>
-    <row r="872" spans="2:2" ht="12">
+    <row r="872" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B872" s="6"/>
     </row>
-    <row r="873" spans="2:2" ht="12">
+    <row r="873" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B873" s="6"/>
     </row>
-    <row r="874" spans="2:2" ht="12">
+    <row r="874" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B874" s="6"/>
     </row>
-    <row r="875" spans="2:2" ht="12">
+    <row r="875" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B875" s="6"/>
     </row>
-    <row r="876" spans="2:2" ht="12">
+    <row r="876" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B876" s="6"/>
     </row>
-    <row r="877" spans="2:2" ht="12">
+    <row r="877" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B877" s="6"/>
     </row>
-    <row r="878" spans="2:2" ht="12">
+    <row r="878" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B878" s="6"/>
     </row>
-    <row r="879" spans="2:2" ht="12">
+    <row r="879" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B879" s="6"/>
     </row>
-    <row r="880" spans="2:2" ht="12">
+    <row r="880" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B880" s="6"/>
     </row>
-    <row r="881" spans="2:2" ht="12">
+    <row r="881" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B881" s="6"/>
     </row>
-    <row r="882" spans="2:2" ht="12">
+    <row r="882" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B882" s="6"/>
     </row>
-    <row r="883" spans="2:2" ht="12">
+    <row r="883" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B883" s="6"/>
     </row>
-    <row r="884" spans="2:2" ht="12">
+    <row r="884" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B884" s="6"/>
     </row>
-    <row r="885" spans="2:2" ht="12">
+    <row r="885" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B885" s="6"/>
     </row>
-    <row r="886" spans="2:2" ht="12">
+    <row r="886" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B886" s="6"/>
     </row>
-    <row r="887" spans="2:2" ht="12">
+    <row r="887" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B887" s="6"/>
     </row>
-    <row r="888" spans="2:2" ht="12">
+    <row r="888" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B888" s="6"/>
     </row>
-    <row r="889" spans="2:2" ht="12">
+    <row r="889" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B889" s="6"/>
     </row>
-    <row r="890" spans="2:2" ht="12">
+    <row r="890" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B890" s="6"/>
     </row>
-    <row r="891" spans="2:2" ht="12">
+    <row r="891" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B891" s="6"/>
     </row>
-    <row r="892" spans="2:2" ht="12">
+    <row r="892" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B892" s="6"/>
     </row>
-    <row r="893" spans="2:2" ht="12">
+    <row r="893" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B893" s="6"/>
     </row>
-    <row r="894" spans="2:2" ht="12">
+    <row r="894" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B894" s="6"/>
     </row>
-    <row r="895" spans="2:2" ht="12">
+    <row r="895" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B895" s="6"/>
     </row>
-    <row r="896" spans="2:2" ht="12">
+    <row r="896" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B896" s="6"/>
     </row>
-    <row r="897" spans="2:2" ht="12">
+    <row r="897" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B897" s="6"/>
     </row>
-    <row r="898" spans="2:2" ht="12">
+    <row r="898" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B898" s="6"/>
     </row>
-    <row r="899" spans="2:2" ht="12">
+    <row r="899" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B899" s="6"/>
     </row>
-    <row r="900" spans="2:2" ht="12">
+    <row r="900" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B900" s="6"/>
     </row>
-    <row r="901" spans="2:2" ht="12">
+    <row r="901" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B901" s="6"/>
     </row>
-    <row r="902" spans="2:2" ht="12">
+    <row r="902" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B902" s="6"/>
     </row>
-    <row r="903" spans="2:2" ht="12">
+    <row r="903" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B903" s="6"/>
     </row>
-    <row r="904" spans="2:2" ht="12">
+    <row r="904" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B904" s="6"/>
     </row>
-    <row r="905" spans="2:2" ht="12">
+    <row r="905" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B905" s="6"/>
     </row>
-    <row r="906" spans="2:2" ht="12">
+    <row r="906" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B906" s="6"/>
     </row>
-    <row r="907" spans="2:2" ht="12">
+    <row r="907" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B907" s="6"/>
     </row>
-    <row r="908" spans="2:2" ht="12">
+    <row r="908" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B908" s="6"/>
     </row>
-    <row r="909" spans="2:2" ht="12">
+    <row r="909" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B909" s="6"/>
     </row>
-    <row r="910" spans="2:2" ht="12">
+    <row r="910" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B910" s="6"/>
     </row>
-    <row r="911" spans="2:2" ht="12">
+    <row r="911" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B911" s="6"/>
     </row>
-    <row r="912" spans="2:2" ht="12">
+    <row r="912" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B912" s="6"/>
     </row>
-    <row r="913" spans="2:2" ht="12">
+    <row r="913" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B913" s="6"/>
     </row>
-    <row r="914" spans="2:2" ht="12">
+    <row r="914" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B914" s="6"/>
     </row>
-    <row r="915" spans="2:2" ht="12">
+    <row r="915" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B915" s="6"/>
     </row>
-    <row r="916" spans="2:2" ht="12">
+    <row r="916" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B916" s="6"/>
     </row>
-    <row r="917" spans="2:2" ht="12">
+    <row r="917" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B917" s="6"/>
     </row>
-    <row r="918" spans="2:2" ht="12">
+    <row r="918" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B918" s="6"/>
     </row>
-    <row r="919" spans="2:2" ht="12">
+    <row r="919" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B919" s="6"/>
     </row>
-    <row r="920" spans="2:2" ht="12">
+    <row r="920" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B920" s="6"/>
     </row>
-    <row r="921" spans="2:2" ht="12">
+    <row r="921" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B921" s="6"/>
     </row>
-    <row r="922" spans="2:2" ht="12">
+    <row r="922" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B922" s="6"/>
     </row>
-    <row r="923" spans="2:2" ht="12">
+    <row r="923" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B923" s="6"/>
     </row>
-    <row r="924" spans="2:2" ht="12">
+    <row r="924" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B924" s="6"/>
     </row>
-    <row r="925" spans="2:2" ht="12">
+    <row r="925" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B925" s="6"/>
     </row>
-    <row r="926" spans="2:2" ht="12">
+    <row r="926" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B926" s="6"/>
     </row>
-    <row r="927" spans="2:2" ht="12">
+    <row r="927" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B927" s="6"/>
     </row>
-    <row r="928" spans="2:2" ht="12">
+    <row r="928" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B928" s="6"/>
     </row>
-    <row r="929" spans="2:2" ht="12">
+    <row r="929" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B929" s="6"/>
     </row>
-    <row r="930" spans="2:2" ht="12">
+    <row r="930" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B930" s="6"/>
     </row>
-    <row r="931" spans="2:2" ht="12">
+    <row r="931" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B931" s="6"/>
     </row>
-    <row r="932" spans="2:2" ht="12">
+    <row r="932" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B932" s="6"/>
     </row>
-    <row r="933" spans="2:2" ht="12">
+    <row r="933" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B933" s="6"/>
     </row>
-    <row r="934" spans="2:2" ht="12">
+    <row r="934" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B934" s="6"/>
     </row>
-    <row r="935" spans="2:2" ht="12">
+    <row r="935" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B935" s="6"/>
     </row>
-    <row r="936" spans="2:2" ht="12">
+    <row r="936" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B936" s="6"/>
     </row>
-    <row r="937" spans="2:2" ht="12">
+    <row r="937" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B937" s="6"/>
     </row>
-    <row r="938" spans="2:2" ht="12">
+    <row r="938" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B938" s="6"/>
     </row>
-    <row r="939" spans="2:2" ht="12">
+    <row r="939" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B939" s="6"/>
     </row>
-    <row r="940" spans="2:2" ht="12">
+    <row r="940" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B940" s="6"/>
     </row>
-    <row r="941" spans="2:2" ht="12">
+    <row r="941" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B941" s="6"/>
     </row>
-    <row r="942" spans="2:2" ht="12">
+    <row r="942" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B942" s="6"/>
     </row>
-    <row r="943" spans="2:2" ht="12">
+    <row r="943" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B943" s="6"/>
     </row>
-    <row r="944" spans="2:2" ht="12">
+    <row r="944" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B944" s="6"/>
     </row>
-    <row r="945" spans="2:2" ht="12">
+    <row r="945" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B945" s="6"/>
     </row>
-    <row r="946" spans="2:2" ht="12">
+    <row r="946" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B946" s="6"/>
     </row>
-    <row r="947" spans="2:2" ht="12">
+    <row r="947" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B947" s="6"/>
     </row>
-    <row r="948" spans="2:2" ht="12">
+    <row r="948" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B948" s="6"/>
     </row>
-    <row r="949" spans="2:2" ht="12">
+    <row r="949" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B949" s="6"/>
     </row>
-    <row r="950" spans="2:2" ht="12">
+    <row r="950" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B950" s="6"/>
     </row>
-    <row r="951" spans="2:2" ht="12">
+    <row r="951" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B951" s="6"/>
     </row>
-    <row r="952" spans="2:2" ht="12">
+    <row r="952" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B952" s="6"/>
     </row>
-    <row r="953" spans="2:2" ht="12">
+    <row r="953" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B953" s="6"/>
     </row>
-    <row r="954" spans="2:2" ht="12">
+    <row r="954" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B954" s="6"/>
     </row>
-    <row r="955" spans="2:2" ht="12">
+    <row r="955" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B955" s="6"/>
     </row>
-    <row r="956" spans="2:2" ht="12">
+    <row r="956" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B956" s="6"/>
     </row>
-    <row r="957" spans="2:2" ht="12">
+    <row r="957" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B957" s="6"/>
     </row>
-    <row r="958" spans="2:2" ht="12">
+    <row r="958" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B958" s="6"/>
     </row>
-    <row r="959" spans="2:2" ht="12">
+    <row r="959" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B959" s="6"/>
     </row>
-    <row r="960" spans="2:2" ht="12">
+    <row r="960" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B960" s="6"/>
     </row>
-    <row r="961" spans="2:2" ht="12">
+    <row r="961" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B961" s="6"/>
     </row>
-    <row r="962" spans="2:2" ht="12">
+    <row r="962" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B962" s="6"/>
     </row>
-    <row r="963" spans="2:2" ht="12">
+    <row r="963" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B963" s="6"/>
     </row>
-    <row r="964" spans="2:2" ht="12">
+    <row r="964" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B964" s="6"/>
     </row>
-    <row r="965" spans="2:2" ht="12">
+    <row r="965" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B965" s="6"/>
     </row>
-    <row r="966" spans="2:2" ht="12">
+    <row r="966" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B966" s="6"/>
     </row>
-    <row r="967" spans="2:2" ht="12">
+    <row r="967" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B967" s="6"/>
     </row>
-    <row r="968" spans="2:2" ht="12">
+    <row r="968" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B968" s="6"/>
     </row>
-    <row r="969" spans="2:2" ht="12">
+    <row r="969" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B969" s="6"/>
     </row>
-    <row r="970" spans="2:2" ht="12">
+    <row r="970" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B970" s="6"/>
     </row>
-    <row r="971" spans="2:2" ht="12">
+    <row r="971" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B971" s="6"/>
     </row>
-    <row r="972" spans="2:2" ht="12">
+    <row r="972" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B972" s="6"/>
     </row>
-    <row r="973" spans="2:2" ht="12">
+    <row r="973" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B973" s="6"/>
     </row>
-    <row r="974" spans="2:2" ht="12">
+    <row r="974" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B974" s="6"/>
     </row>
-    <row r="975" spans="2:2" ht="12">
+    <row r="975" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B975" s="6"/>
     </row>
-    <row r="976" spans="2:2" ht="12">
+    <row r="976" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B976" s="6"/>
     </row>
-    <row r="977" spans="2:2" ht="12">
+    <row r="977" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B977" s="6"/>
     </row>
-    <row r="978" spans="2:2" ht="12">
+    <row r="978" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B978" s="6"/>
     </row>
-    <row r="979" spans="2:2" ht="12">
+    <row r="979" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B979" s="6"/>
     </row>
-    <row r="980" spans="2:2" ht="12">
+    <row r="980" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B980" s="6"/>
     </row>
-    <row r="981" spans="2:2" ht="12">
+    <row r="981" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B981" s="6"/>
     </row>
-    <row r="982" spans="2:2" ht="12">
+    <row r="982" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B982" s="6"/>
     </row>
-    <row r="983" spans="2:2" ht="12">
+    <row r="983" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B983" s="6"/>
     </row>
-    <row r="984" spans="2:2" ht="12">
+    <row r="984" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B984" s="6"/>
     </row>
-    <row r="985" spans="2:2" ht="12">
+    <row r="985" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B985" s="6"/>
     </row>
-    <row r="986" spans="2:2" ht="12">
+    <row r="986" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B986" s="6"/>
     </row>
-    <row r="987" spans="2:2" ht="12">
+    <row r="987" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B987" s="6"/>
     </row>
-    <row r="988" spans="2:2" ht="12">
+    <row r="988" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B988" s="6"/>
     </row>
-    <row r="989" spans="2:2" ht="12">
+    <row r="989" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B989" s="6"/>
     </row>
   </sheetData>
@@ -4760,9 +4776,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:26" ht="15.75" customHeight="1">
+    <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>31</v>
       </c>
@@ -4800,7 +4816,7 @@
       <c r="Y1" s="11"/>
       <c r="Z1" s="11"/>
     </row>
-    <row r="2" spans="1:26" ht="15.75" customHeight="1">
+    <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
         <v>36</v>
       </c>
@@ -4832,7 +4848,7 @@
       <c r="Y2" s="11"/>
       <c r="Z2" s="11"/>
     </row>
-    <row r="3" spans="1:26" ht="15.75" customHeight="1">
+    <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
         <v>38</v>
       </c>
@@ -4864,7 +4880,7 @@
       <c r="Y3" s="11"/>
       <c r="Z3" s="11"/>
     </row>
-    <row r="4" spans="1:26" ht="15.75" customHeight="1">
+    <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
         <v>40</v>
       </c>
@@ -4898,7 +4914,7 @@
       <c r="Y4" s="11"/>
       <c r="Z4" s="11"/>
     </row>
-    <row r="5" spans="1:26" ht="15.75" customHeight="1">
+    <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
         <v>43</v>
       </c>
@@ -4932,7 +4948,7 @@
       <c r="Y5" s="11"/>
       <c r="Z5" s="11"/>
     </row>
-    <row r="6" spans="1:26" ht="15.75" customHeight="1">
+    <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
         <v>46</v>
       </c>
@@ -4966,7 +4982,7 @@
       <c r="Y6" s="11"/>
       <c r="Z6" s="11"/>
     </row>
-    <row r="7" spans="1:26" ht="15.75" customHeight="1">
+    <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>49</v>
       </c>
@@ -4986,7 +5002,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="8" spans="1:26" ht="15.75" customHeight="1">
+    <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="14" t="s">
         <v>55</v>
       </c>

</xml_diff>